<commit_message>
Corrected computation and interpolation error
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -476,10 +476,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Franklin, WV</t>
-        </is>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>79.33806</v>
@@ -488,29 +486,27 @@
         <v>38.63556</v>
       </c>
       <c r="D2" t="n">
-        <v>0.06729834152203831</v>
+        <v>0.1222663421630673</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6758975143520155</v>
+        <v>0.4463349292960735</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.09124506723702636</v>
+        <v>-0.101348779735704</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5704621538668957</v>
+        <v>0.5283631798708452</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3111801024738692</v>
+        <v>0.3012624858660398</v>
       </c>
       <c r="I2" t="n">
-        <v>0.04766083382010095</v>
+        <v>0.05560748976738104</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Petersburg, WV</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B3" t="n">
         <v>79.17610999999999</v>
@@ -519,29 +515,27 @@
         <v>38.99111</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0252164027726736</v>
+        <v>0.06918130648859001</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8756427062593654</v>
+        <v>0.6673463000276509</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.1512129329831112</v>
+        <v>-0.158334081747683</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3453056013696145</v>
+        <v>0.32279291759125</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3559471620602919</v>
+        <v>0.3501610335207801</v>
       </c>
       <c r="I3" t="n">
-        <v>0.02236756924546843</v>
+        <v>0.02480856298740221</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Brandywine, WV</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B4" t="n">
         <v>79.24666999999999</v>
@@ -550,29 +544,27 @@
         <v>38.63139</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.0138593690840669</v>
+        <v>0.04793589244181456</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9314641220022912</v>
+        <v>0.765994442827437</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.1429213382541503</v>
+        <v>-0.1533061988016138</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3726982694250711</v>
+        <v>0.3385904288116929</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1669421156252396</v>
+        <v>0.1605040844743924</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2968386650454003</v>
+        <v>0.3161199627949248</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Stokesville, VA</t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B5" t="n">
         <v>79.23917</v>
@@ -581,29 +573,27 @@
         <v>38.335</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1492507176017555</v>
+        <v>0.2037746548542168</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3516738934270134</v>
+        <v>0.2012843192929921</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.09190170105041261</v>
+        <v>-0.1030844758157276</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5676801780991874</v>
+        <v>0.521287410410006</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1536714933185467</v>
+        <v>0.1444505100508748</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3374268804766944</v>
+        <v>0.3675515323530053</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Bacova, VA</t>
-        </is>
+      <c r="A6" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B6" t="n">
         <v>79.88167</v>
@@ -612,29 +602,27 @@
         <v>38.04222</v>
       </c>
       <c r="D6" t="n">
-        <v>0.04784277295449189</v>
+        <v>0.1465907324647266</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7664363001252992</v>
+        <v>0.3604200454422758</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.1776344952207985</v>
+        <v>-0.1855485264278399</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2665228772064374</v>
+        <v>0.2454517194232228</v>
       </c>
       <c r="H6" t="n">
-        <v>0.1842052799626536</v>
+        <v>0.1793885938969529</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2489465710874465</v>
+        <v>0.2617525712827215</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Sunrise, VA</t>
-        </is>
+      <c r="A7" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B7" t="n">
         <v>79.76889</v>
@@ -643,29 +631,27 @@
         <v>38.24528</v>
       </c>
       <c r="D7" t="n">
-        <v>0.009348482525955708</v>
+        <v>0.1134287231409957</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9537410424983354</v>
+        <v>0.4801128018386313</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.2362936230414762</v>
+        <v>-0.2423699499271562</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1369141587288243</v>
+        <v>0.1268113470656143</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3092035300220394</v>
+        <v>0.3070877608110859</v>
       </c>
       <c r="I7" t="n">
-        <v>0.04916667447791636</v>
+        <v>0.05082082595474559</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Hot Springs, VA</t>
-        </is>
+      <c r="A8" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B8" t="n">
         <v>79.94944</v>
@@ -674,29 +660,27 @@
         <v>37.94833</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1397348186997984</v>
+        <v>0.2105429803284323</v>
       </c>
       <c r="E8" t="n">
-        <v>0.3835600732417203</v>
+        <v>0.1863984389850216</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.08760043048978669</v>
+        <v>-0.091823138545535</v>
       </c>
       <c r="G8" t="n">
-        <v>0.5860157711975431</v>
+        <v>0.5680126967637498</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1754294896216742</v>
+        <v>0.1708092061995602</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2726004838172222</v>
+        <v>0.2856285980746613</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Covington, VA</t>
-        </is>
+      <c r="A9" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B9" t="n">
         <v>80.04722</v>
@@ -705,29 +689,27 @@
         <v>37.80278</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.008001226819858334</v>
+        <v>0.1001110550319311</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9604019424489771</v>
+        <v>0.533437455683532</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.1269267398518684</v>
+        <v>-0.1310560764600157</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4290607420933636</v>
+        <v>0.4140723106154279</v>
       </c>
       <c r="H9" t="n">
-        <v>0.1227525905514282</v>
+        <v>0.1196083672353616</v>
       </c>
       <c r="I9" t="n">
-        <v>0.4445150306740134</v>
+        <v>0.4563547259192757</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Covington, VA1</t>
-        </is>
+      <c r="A10" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B10" t="n">
         <v>80.00082999999999</v>
@@ -736,29 +718,27 @@
         <v>37.78861</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1078903003135303</v>
+        <v>0.2092068831004232</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5019436021999824</v>
+        <v>0.1892731848998503</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.06126534712797704</v>
+        <v>-0.06607046532172667</v>
       </c>
       <c r="G10" t="n">
-        <v>0.7035626220789143</v>
+        <v>0.6814955430825904</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1467782701361069</v>
+        <v>0.1409114446891574</v>
       </c>
       <c r="I10" t="n">
-        <v>0.3597991500931508</v>
+        <v>0.3795278401432624</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Covington, VA2</t>
-        </is>
+      <c r="A11" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B11" t="n">
         <v>80.0425</v>
@@ -767,29 +747,27 @@
         <v>37.72889</v>
       </c>
       <c r="D11" t="n">
-        <v>0.08640766058688173</v>
+        <v>0.164361212932865</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5911466877368159</v>
+        <v>0.3044754376257463</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0587916502589448</v>
+        <v>-0.06415997329838764</v>
       </c>
       <c r="G11" t="n">
-        <v>0.7150184857151616</v>
+        <v>0.690239206944834</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1254886111673731</v>
+        <v>0.1201208837896621</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4343510381220569</v>
+        <v>0.4544132853812123</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>Williamsville, VA</t>
-        </is>
+      <c r="A12" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B12" t="n">
         <v>79.57028</v>
@@ -798,29 +776,27 @@
         <v>38.19528</v>
       </c>
       <c r="D12" t="n">
-        <v>0.170852367827095</v>
+        <v>0.2147405869476079</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2855050526598142</v>
+        <v>0.1775688782213128</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.0377072723147092</v>
+        <v>-0.0453489432058654</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8149378189382566</v>
+        <v>0.7782964049606389</v>
       </c>
       <c r="H12" t="n">
-        <v>0.2920713770626272</v>
+        <v>0.282738358363616</v>
       </c>
       <c r="I12" t="n">
-        <v>0.06388708859952534</v>
+        <v>0.07326639147951426</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>Clifton Forge, VA</t>
-        </is>
+      <c r="A13" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B13" t="n">
         <v>79.75972</v>
@@ -829,29 +805,27 @@
         <v>37.79167</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.01403386207095322</v>
+        <v>0.06154512595056418</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9306033190055732</v>
+        <v>0.7022709521448876</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.1720451030604882</v>
+        <v>-0.1796817618513676</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2821047131856534</v>
+        <v>0.2609608611582873</v>
       </c>
       <c r="H13" t="n">
-        <v>0.1472578346463939</v>
+        <v>0.1436457207728654</v>
       </c>
       <c r="I13" t="n">
-        <v>0.3582143574286503</v>
+        <v>0.3702548880022567</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>Lick Run, VA</t>
-        </is>
+      <c r="A14" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B14" t="n">
         <v>79.78471999999999</v>
@@ -860,29 +834,27 @@
         <v>37.77361</v>
       </c>
       <c r="D14" t="n">
-        <v>0.07472458862070072</v>
+        <v>0.1639850610155492</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6424155931214424</v>
+        <v>0.3055988239595103</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.086997144546125</v>
+        <v>-0.09323464075638996</v>
       </c>
       <c r="G14" t="n">
-        <v>0.5886084342885992</v>
+        <v>0.5620521581679291</v>
       </c>
       <c r="H14" t="n">
-        <v>0.162097317187728</v>
+        <v>0.1561995593386685</v>
       </c>
       <c r="I14" t="n">
-        <v>0.3112764467260338</v>
+        <v>0.3294422126045209</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>New Castle, VA</t>
-        </is>
+      <c r="A15" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B15" t="n">
         <v>80.10693999999999</v>
@@ -891,29 +863,27 @@
         <v>37.50611</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2238780793206508</v>
+        <v>0.242221089606042</v>
       </c>
       <c r="E15" t="n">
-        <v>0.159391583205801</v>
+        <v>0.1270519916116278</v>
       </c>
       <c r="F15" t="n">
-        <v>0.07159229805617297</v>
+        <v>0.06968732478824614</v>
       </c>
       <c r="G15" t="n">
-        <v>0.6564575712166424</v>
+        <v>0.6650552948797606</v>
       </c>
       <c r="H15" t="n">
-        <v>0.2155983481305875</v>
+        <v>0.2088931334292092</v>
       </c>
       <c r="I15" t="n">
-        <v>0.1758020629151686</v>
+        <v>0.1899527763716995</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Parr, VA</t>
-        </is>
+      <c r="A16" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B16" t="n">
         <v>79.90889</v>
@@ -922,29 +892,27 @@
         <v>37.66583</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2182534674417697</v>
+        <v>0.2503063039877526</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1704129690647458</v>
+        <v>0.1144690425986356</v>
       </c>
       <c r="F16" t="n">
-        <v>0.05351234072800208</v>
+        <v>0.05116729861016329</v>
       </c>
       <c r="G16" t="n">
-        <v>0.739671850320217</v>
+        <v>0.7507074468943383</v>
       </c>
       <c r="H16" t="n">
-        <v>0.1992451909390401</v>
+        <v>0.1924578600475391</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2116999315882634</v>
+        <v>0.227998530925218</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>Catawba, VA</t>
-        </is>
+      <c r="A17" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B17" t="n">
         <v>80.00556</v>
@@ -953,29 +921,27 @@
         <v>37.46806</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2427016307272414</v>
+        <v>0.2348305550882017</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1262763848543938</v>
+        <v>0.1394334621132922</v>
       </c>
       <c r="F17" t="n">
-        <v>0.09308614218078924</v>
+        <v>0.08990462043921008</v>
       </c>
       <c r="G17" t="n">
-        <v>0.5626778735358272</v>
+        <v>0.5761605491446717</v>
       </c>
       <c r="H17" t="n">
-        <v>0.1603386099880324</v>
+        <v>0.1521378696645656</v>
       </c>
       <c r="I17" t="n">
-        <v>0.3166257246465521</v>
+        <v>0.3423284190778705</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Buchanan, VA</t>
-        </is>
+      <c r="A18" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B18" t="n">
         <v>79.67917</v>
@@ -984,29 +950,27 @@
         <v>37.53056</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1137185068512036</v>
+        <v>0.1746260386175583</v>
       </c>
       <c r="E18" t="n">
-        <v>0.4789844295945208</v>
+        <v>0.2748374849744579</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.06610035804580525</v>
+        <v>-0.07051398506630964</v>
       </c>
       <c r="G18" t="n">
-        <v>0.6813590569015952</v>
+        <v>0.661319044289432</v>
       </c>
       <c r="H18" t="n">
-        <v>0.1738667391242813</v>
+        <v>0.168898998707394</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2769625959010902</v>
+        <v>0.2911311322761961</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>Rockbridge Baths, VA</t>
-        </is>
+      <c r="A19" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B19" t="n">
         <v>79.42222</v>
@@ -1015,29 +979,27 @@
         <v>37.90722</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.04323774581499815</v>
+        <v>0.04106695209216875</v>
       </c>
       <c r="E19" t="n">
-        <v>0.7883758476040231</v>
+        <v>0.7987754289034322</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.196137247424106</v>
+        <v>-0.2010899483791829</v>
       </c>
       <c r="G19" t="n">
-        <v>0.219059685611971</v>
+        <v>0.2074136008242457</v>
       </c>
       <c r="H19" t="n">
-        <v>0.04814378962996164</v>
+        <v>0.04822865706727394</v>
       </c>
       <c r="I19" t="n">
-        <v>0.7650082228848909</v>
+        <v>0.7646057349733906</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>Lexington, VA</t>
-        </is>
+      <c r="A20" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B20" t="n">
         <v>79.44333</v>
@@ -1046,29 +1008,27 @@
         <v>37.82556</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01628058208274138</v>
+        <v>0.0916233177738958</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9195271831499017</v>
+        <v>0.5688588487435837</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.1286540968015076</v>
+        <v>-0.1312577288285174</v>
       </c>
       <c r="G20" t="n">
-        <v>0.4227543471195597</v>
+        <v>0.4133480750575992</v>
       </c>
       <c r="H20" t="n">
-        <v>0.002560808117075153</v>
+        <v>0.002377749709099805</v>
       </c>
       <c r="I20" t="n">
-        <v>0.9873220741836941</v>
+        <v>0.9882282853318953</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>Buena Vista, VA</t>
-        </is>
+      <c r="A21" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B21" t="n">
         <v>79.39167</v>
@@ -1077,29 +1037,27 @@
         <v>37.7625</v>
       </c>
       <c r="D21" t="n">
-        <v>0.007038119567629859</v>
+        <v>0.07436999231603043</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9651652479832675</v>
+        <v>0.6439992041400902</v>
       </c>
       <c r="F21" t="n">
-        <v>-0.1219827833340898</v>
+        <v>-0.1261535164290962</v>
       </c>
       <c r="G21" t="n">
-        <v>0.447398093298022</v>
+        <v>0.431900632609663</v>
       </c>
       <c r="H21" t="n">
-        <v>0.08531432863022223</v>
+        <v>0.08320207005194005</v>
       </c>
       <c r="I21" t="n">
-        <v>0.5958672087166584</v>
+        <v>0.6050334229503453</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>Holcomb Rock, VA</t>
-        </is>
+      <c r="A22" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B22" t="n">
         <v>79.26278000000001</v>
@@ -1108,29 +1066,27 @@
         <v>37.50111</v>
       </c>
       <c r="D22" t="n">
-        <v>0.01061710032381728</v>
+        <v>0.07488159920751677</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9474717615134466</v>
+        <v>0.6417148890694666</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.1269546603825919</v>
+        <v>-0.131089451732876</v>
       </c>
       <c r="G22" t="n">
-        <v>0.4289583912735363</v>
+        <v>0.4139523933486098</v>
       </c>
       <c r="H22" t="n">
-        <v>0.1380742297411116</v>
+        <v>0.1357329653092354</v>
       </c>
       <c r="I22" t="n">
-        <v>0.3892935078571778</v>
+        <v>0.3974616348354016</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>Piney River, VA</t>
-        </is>
+      <c r="A23" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B23" t="n">
         <v>79.02778000000001</v>
@@ -1139,29 +1095,27 @@
         <v>37.70222</v>
       </c>
       <c r="D23" t="n">
-        <v>0.02138720833454983</v>
+        <v>0.06384818893730092</v>
       </c>
       <c r="E23" t="n">
-        <v>0.8944109153127437</v>
+        <v>0.6916699515162754</v>
       </c>
       <c r="F23" t="n">
-        <v>-0.1350492495230945</v>
+        <v>-0.1382155592385337</v>
       </c>
       <c r="G23" t="n">
-        <v>0.3998655557521736</v>
+        <v>0.388803604871867</v>
       </c>
       <c r="H23" t="n">
-        <v>0.1283993528454279</v>
+        <v>0.1274400472098834</v>
       </c>
       <c r="I23" t="n">
-        <v>0.4236810961730113</v>
+        <v>0.4271812460299097</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>Shawsville, VA</t>
-        </is>
+      <c r="A24" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B24" t="n">
         <v>80.26667</v>
@@ -1170,29 +1124,27 @@
         <v>37.14</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3406051191941804</v>
+        <v>0.366165251684785</v>
       </c>
       <c r="E24" t="n">
-        <v>0.02932332186731569</v>
+        <v>0.01854666723361252</v>
       </c>
       <c r="F24" t="n">
-        <v>0.1124614099250002</v>
+        <v>0.1110420953837681</v>
       </c>
       <c r="G24" t="n">
-        <v>0.4838894282330399</v>
+        <v>0.4894586817651733</v>
       </c>
       <c r="H24" t="n">
-        <v>0.1953180414424053</v>
+        <v>0.187178632537133</v>
       </c>
       <c r="I24" t="n">
-        <v>0.2210286467298135</v>
+        <v>0.2412551295450372</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>Lafayette, VA</t>
-        </is>
+      <c r="A25" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B25" t="n">
         <v>80.20944</v>
@@ -1201,29 +1153,27 @@
         <v>37.23639</v>
       </c>
       <c r="D25" t="n">
-        <v>0.2885906058408017</v>
+        <v>0.3166379887398568</v>
       </c>
       <c r="E25" t="n">
-        <v>0.06726686371945316</v>
+        <v>0.04369535938993665</v>
       </c>
       <c r="F25" t="n">
-        <v>0.1075018125179651</v>
+        <v>0.1058327580014547</v>
       </c>
       <c r="G25" t="n">
-        <v>0.5034936116864995</v>
+        <v>0.510180419902783</v>
       </c>
       <c r="H25" t="n">
-        <v>0.2148963781794687</v>
+        <v>0.2068065380846656</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1772470391674217</v>
+        <v>0.1945163731486233</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>Roanoke, VA</t>
-        </is>
+      <c r="A26" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B26" t="n">
         <v>79.93889</v>
@@ -1232,29 +1182,27 @@
         <v>37.25833</v>
       </c>
       <c r="D26" t="n">
-        <v>0.3007854732276736</v>
+        <v>0.3328850240196835</v>
       </c>
       <c r="E26" t="n">
-        <v>0.05601491622416221</v>
+        <v>0.03344862391598589</v>
       </c>
       <c r="F26" t="n">
-        <v>0.1094738331510376</v>
+        <v>0.1058369521496104</v>
       </c>
       <c r="G26" t="n">
-        <v>0.4956507336208968</v>
+        <v>0.5101635609456341</v>
       </c>
       <c r="H26" t="n">
-        <v>0.1936690390068409</v>
+        <v>0.1837994185564765</v>
       </c>
       <c r="I26" t="n">
-        <v>0.2250289060964284</v>
+        <v>0.2500090828682152</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>Niagara, VA</t>
-        </is>
+      <c r="A27" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B27" t="n">
         <v>79.87166999999999</v>
@@ -1263,29 +1211,27 @@
         <v>35.255</v>
       </c>
       <c r="D27" t="n">
-        <v>0.3013007697926858</v>
+        <v>0.3270683744826845</v>
       </c>
       <c r="E27" t="n">
-        <v>0.05557489377273213</v>
+        <v>0.03686230362768605</v>
       </c>
       <c r="F27" t="n">
-        <v>0.1304932400940838</v>
+        <v>0.1265959032483973</v>
       </c>
       <c r="G27" t="n">
-        <v>0.4160975532204284</v>
+        <v>0.4302745579185775</v>
       </c>
       <c r="H27" t="n">
-        <v>0.1865122584428442</v>
+        <v>0.1758747784029902</v>
       </c>
       <c r="I27" t="n">
-        <v>0.2429647564583278</v>
+        <v>0.2713658631045977</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>Dundee, VA</t>
-        </is>
+      <c r="A28" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B28" t="n">
         <v>79.86833</v>
@@ -1294,29 +1240,27 @@
         <v>37.2275</v>
       </c>
       <c r="D28" t="n">
-        <v>0.3483303568898826</v>
+        <v>0.3702575390459191</v>
       </c>
       <c r="E28" t="n">
-        <v>0.02562554015264454</v>
+        <v>0.01717854333628179</v>
       </c>
       <c r="F28" t="n">
-        <v>0.1357261428091826</v>
+        <v>0.1305543282270946</v>
       </c>
       <c r="G28" t="n">
-        <v>0.3974855810673902</v>
+        <v>0.415877469626714</v>
       </c>
       <c r="H28" t="n">
-        <v>0.1701982991608242</v>
+        <v>0.158378679107412</v>
       </c>
       <c r="I28" t="n">
-        <v>0.2873809758561823</v>
+        <v>0.3226548947875838</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>Rocky Mount, VA</t>
-        </is>
+      <c r="A29" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B29" t="n">
         <v>79.84444000000001</v>
@@ -1325,29 +1269,27 @@
         <v>37.045</v>
       </c>
       <c r="D29" t="n">
-        <v>0.3305817188303538</v>
+        <v>0.3445186839593103</v>
       </c>
       <c r="E29" t="n">
-        <v>0.03476792540200613</v>
+        <v>0.02739844191271793</v>
       </c>
       <c r="F29" t="n">
-        <v>0.07281745676282703</v>
+        <v>0.06787289505146341</v>
       </c>
       <c r="G29" t="n">
-        <v>0.6509509813283922</v>
+        <v>0.6732839386261732</v>
       </c>
       <c r="H29" t="n">
-        <v>0.1829197018658163</v>
+        <v>0.1734091459437307</v>
       </c>
       <c r="I29" t="n">
-        <v>0.2523225449739455</v>
+        <v>0.2782484796731109</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>Sandy Level, VA</t>
-        </is>
+      <c r="A30" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B30" t="n">
         <v>79.52500000000001</v>
@@ -1356,29 +1298,27 @@
         <v>36.94583</v>
       </c>
       <c r="D30" t="n">
-        <v>0.200449955748481</v>
+        <v>0.2611183064445699</v>
       </c>
       <c r="E30" t="n">
-        <v>0.2088937269170725</v>
+        <v>0.09914443219426383</v>
       </c>
       <c r="F30" t="n">
-        <v>-0.0823891792739006</v>
+        <v>-0.08584195486773358</v>
       </c>
       <c r="G30" t="n">
-        <v>0.6085770978666136</v>
+        <v>0.5935870912471931</v>
       </c>
       <c r="H30" t="n">
-        <v>0.0734081154273156</v>
+        <v>0.07006143845882352</v>
       </c>
       <c r="I30" t="n">
-        <v>0.6483027132649118</v>
+        <v>0.6633634188715578</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
-        <is>
-          <t>Huddleston, VA</t>
-        </is>
+      <c r="A31" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B31" t="n">
         <v>79.52056</v>
@@ -1387,29 +1327,27 @@
         <v>37.17306</v>
       </c>
       <c r="D31" t="n">
-        <v>0.1725303865122301</v>
+        <v>0.2489282093254854</v>
       </c>
       <c r="E31" t="n">
-        <v>0.2807288158957143</v>
+        <v>0.1165443232646759</v>
       </c>
       <c r="F31" t="n">
-        <v>-0.07759550065758931</v>
+        <v>-0.07860496742477273</v>
       </c>
       <c r="G31" t="n">
-        <v>0.6296522075295165</v>
+        <v>0.6251892490020626</v>
       </c>
       <c r="H31" t="n">
-        <v>0.05670108177429297</v>
+        <v>0.05549382079036201</v>
       </c>
       <c r="I31" t="n">
-        <v>0.724748506175825</v>
+        <v>0.7303870292423437</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>Evington, VA</t>
-        </is>
+      <c r="A32" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B32" t="n">
         <v>79.30389</v>
@@ -1418,29 +1356,27 @@
         <v>37.20833</v>
       </c>
       <c r="D32" t="n">
-        <v>0.04982814610761917</v>
+        <v>0.1340237725084864</v>
       </c>
       <c r="E32" t="n">
-        <v>0.7570316164114747</v>
+        <v>0.4034868025288382</v>
       </c>
       <c r="F32" t="n">
-        <v>-0.1715651896466455</v>
+        <v>-0.1724076348568667</v>
       </c>
       <c r="G32" t="n">
-        <v>0.2834696995325545</v>
+        <v>0.2810764324175494</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.01055395276689875</v>
+        <v>-0.00790748436181931</v>
       </c>
       <c r="I32" t="n">
-        <v>0.9477837545807258</v>
+        <v>0.960865513910683</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="inlineStr">
-        <is>
-          <t>Francisco, NC</t>
-        </is>
+      <c r="A33" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B33" t="n">
         <v>80.30306</v>
@@ -1449,29 +1385,27 @@
         <v>36.515</v>
       </c>
       <c r="D33" t="n">
-        <v>0.2206564029571882</v>
+        <v>0.1523433900652428</v>
       </c>
       <c r="E33" t="n">
-        <v>0.1656391810789122</v>
+        <v>0.3416690392404718</v>
       </c>
       <c r="F33" t="n">
-        <v>0.271644893410507</v>
+        <v>0.2663541845369223</v>
       </c>
       <c r="G33" t="n">
-        <v>0.08578605128193922</v>
+        <v>0.09231361588511666</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.08348050863265202</v>
+        <v>-0.09631548906121098</v>
       </c>
       <c r="I33" t="n">
-        <v>0.6038216591809833</v>
+        <v>0.5491441072276525</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="inlineStr">
-        <is>
-          <t>Nettleridge, VA</t>
-        </is>
+      <c r="A34" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B34" t="n">
         <v>80.12972000000001</v>
@@ -1480,29 +1414,27 @@
         <v>36.57083</v>
       </c>
       <c r="D34" t="n">
-        <v>0.1377754054560942</v>
+        <v>0.1702800020007368</v>
       </c>
       <c r="E34" t="n">
-        <v>0.3903305365487489</v>
+        <v>0.2871462095316255</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.06716383569718945</v>
+        <v>-0.06381353265830332</v>
       </c>
       <c r="G34" t="n">
-        <v>0.6765099093445873</v>
+        <v>0.691829050866992</v>
       </c>
       <c r="H34" t="n">
-        <v>0.2335345275229594</v>
+        <v>0.2353002555425001</v>
       </c>
       <c r="I34" t="n">
-        <v>0.1416936286188921</v>
+        <v>0.1386209615323759</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>Spencer, VA</t>
-        </is>
+      <c r="A35" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B35" t="n">
         <v>79.9875</v>
@@ -1511,29 +1443,27 @@
         <v>36.56806</v>
       </c>
       <c r="D35" t="n">
-        <v>0.1273391457918712</v>
+        <v>0.1792263195384918</v>
       </c>
       <c r="E35" t="n">
-        <v>0.4275503362772681</v>
+        <v>0.2621914838114301</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.1067074764977276</v>
+        <v>-0.1067999546146352</v>
       </c>
       <c r="G35" t="n">
-        <v>0.5066704390271028</v>
+        <v>0.5063000666957047</v>
       </c>
       <c r="H35" t="n">
-        <v>0.1905255412427036</v>
+        <v>0.1908665195582265</v>
       </c>
       <c r="I35" t="n">
-        <v>0.2327916166434293</v>
+        <v>0.231940874043401</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>Wentworth, NC</t>
-        </is>
+      <c r="A36" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B36" t="n">
         <v>79.82611</v>
@@ -1542,29 +1472,27 @@
         <v>36.4125</v>
       </c>
       <c r="D36" t="n">
-        <v>0.1306406974026141</v>
+        <v>0.1854858633639483</v>
       </c>
       <c r="E36" t="n">
-        <v>0.4155664181790701</v>
+        <v>0.2456140167036918</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.06882650802392604</v>
+        <v>-0.06983714454148411</v>
       </c>
       <c r="G36" t="n">
-        <v>0.6689544356921446</v>
+        <v>0.6643775589173782</v>
       </c>
       <c r="H36" t="n">
-        <v>0.1861930655965786</v>
+        <v>0.184328506152852</v>
       </c>
       <c r="I36" t="n">
-        <v>0.243786558494238</v>
+        <v>0.2486245763432652</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>Philpott, VA</t>
-        </is>
+      <c r="A37" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B37" t="n">
         <v>80.02500000000001</v>
@@ -1573,29 +1501,27 @@
         <v>36.78056</v>
       </c>
       <c r="D37" t="n">
-        <v>0.3533729991655608</v>
+        <v>0.3620079940544659</v>
       </c>
       <c r="E37" t="n">
-        <v>0.02342754080956493</v>
+        <v>0.02002915810004469</v>
       </c>
       <c r="F37" t="n">
-        <v>0.2107319825822399</v>
+        <v>0.2094736624997905</v>
       </c>
       <c r="G37" t="n">
-        <v>0.1859942987090067</v>
+        <v>0.1886966885911546</v>
       </c>
       <c r="H37" t="n">
-        <v>0.1381525015811835</v>
+        <v>0.1280407429830372</v>
       </c>
       <c r="I37" t="n">
-        <v>0.3890221426526422</v>
+        <v>0.4249876391270267</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>Bassett, VA</t>
-        </is>
+      <c r="A38" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B38" t="n">
         <v>80.00111</v>
@@ -1604,29 +1530,27 @@
         <v>36.77</v>
       </c>
       <c r="D38" t="n">
-        <v>0.304700032155173</v>
+        <v>0.3170137943146583</v>
       </c>
       <c r="E38" t="n">
-        <v>0.05274108217739546</v>
+        <v>0.04343247927447941</v>
       </c>
       <c r="F38" t="n">
-        <v>0.1181537008676797</v>
+        <v>0.1169839006951648</v>
       </c>
       <c r="G38" t="n">
-        <v>0.4618894115070377</v>
+        <v>0.4663662324701746</v>
       </c>
       <c r="H38" t="n">
-        <v>0.1786560307536196</v>
+        <v>0.1710128077494527</v>
       </c>
       <c r="I38" t="n">
-        <v>0.2637378493697932</v>
+        <v>0.2850461153953701</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>Martinsville, VA</t>
-        </is>
+      <c r="A39" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B39" t="n">
         <v>79.88083</v>
@@ -1635,29 +1559,27 @@
         <v>36.66111</v>
       </c>
       <c r="D39" t="n">
-        <v>0.2120671811678784</v>
+        <v>0.2394875124008028</v>
       </c>
       <c r="E39" t="n">
-        <v>0.1831569859845265</v>
+        <v>0.1315319692535822</v>
       </c>
       <c r="F39" t="n">
-        <v>-0.03275895790908458</v>
+        <v>-0.03200432600558507</v>
       </c>
       <c r="G39" t="n">
-        <v>0.8388792650411707</v>
+        <v>0.8425435936900783</v>
       </c>
       <c r="H39" t="n">
-        <v>0.2178758463733007</v>
+        <v>0.2162004291967804</v>
       </c>
       <c r="I39" t="n">
-        <v>0.1711720829815673</v>
+        <v>0.1745694452588338</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>Eden, NC</t>
-        </is>
+      <c r="A40" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B40" t="n">
         <v>79.76555999999999</v>
@@ -1666,29 +1588,27 @@
         <v>36.52556</v>
       </c>
       <c r="D40" t="n">
-        <v>0.154140321414968</v>
+        <v>0.202807246376807</v>
       </c>
       <c r="E40" t="n">
-        <v>0.335937176625435</v>
+        <v>0.2034781411805929</v>
       </c>
       <c r="F40" t="n">
-        <v>-0.06933575288711355</v>
+        <v>-0.07171975065074142</v>
       </c>
       <c r="G40" t="n">
-        <v>0.6666467245368497</v>
+        <v>0.6558838808379254</v>
       </c>
       <c r="H40" t="n">
-        <v>0.179674755364394</v>
+        <v>0.1767235778093892</v>
       </c>
       <c r="I40" t="n">
-        <v>0.2609797638348546</v>
+        <v>0.2690226662389693</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="inlineStr">
-        <is>
-          <t>Danville, VA</t>
-        </is>
+      <c r="A41" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B41" t="n">
         <v>79.50444</v>
@@ -1697,29 +1617,27 @@
         <v>36.61944</v>
       </c>
       <c r="D41" t="n">
-        <v>0.154140321414968</v>
+        <v>0.202807246376807</v>
       </c>
       <c r="E41" t="n">
-        <v>0.335937176625435</v>
+        <v>0.2034781411805929</v>
       </c>
       <c r="F41" t="n">
-        <v>-0.06933575288711355</v>
+        <v>-0.07171975065074142</v>
       </c>
       <c r="G41" t="n">
-        <v>0.6666467245368497</v>
+        <v>0.6558838808379254</v>
       </c>
       <c r="H41" t="n">
-        <v>0.179674755364394</v>
+        <v>0.1767235778093892</v>
       </c>
       <c r="I41" t="n">
-        <v>0.2609797638348546</v>
+        <v>0.2690226662389693</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>Paces, VA</t>
-        </is>
+      <c r="A42" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B42" t="n">
         <v>79.08972</v>
@@ -1728,29 +1646,27 @@
         <v>36.64222</v>
       </c>
       <c r="D42" t="n">
-        <v>0.09721005796666456</v>
+        <v>0.1664184405400278</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5454225820110846</v>
+        <v>0.2983781508994834</v>
       </c>
       <c r="F42" t="n">
-        <v>-0.1206307984654124</v>
+        <v>-0.1226535131170952</v>
       </c>
       <c r="G42" t="n">
-        <v>0.4524861487136608</v>
+        <v>0.4448855207951836</v>
       </c>
       <c r="H42" t="n">
-        <v>0.1852958923224102</v>
+        <v>0.1838952285777231</v>
       </c>
       <c r="I42" t="n">
-        <v>0.2461064833976088</v>
+        <v>0.249757986098348</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="inlineStr">
-        <is>
-          <t>Leasburg, NC</t>
-        </is>
+      <c r="A43" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B43" t="n">
         <v>79.19667</v>
@@ -1759,29 +1675,27 @@
         <v>36.39778</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.08329730982750061</v>
+        <v>-0.01797176447969796</v>
       </c>
       <c r="E43" t="n">
-        <v>0.6046188218890752</v>
+        <v>0.9111995729470568</v>
       </c>
       <c r="F43" t="n">
-        <v>-0.160961975908406</v>
+        <v>-0.1617679059064384</v>
       </c>
       <c r="G43" t="n">
-        <v>0.3147231055782881</v>
+        <v>0.3122739975229081</v>
       </c>
       <c r="H43" t="n">
-        <v>-0.09914079429882923</v>
+        <v>-0.09463103541367664</v>
       </c>
       <c r="I43" t="n">
-        <v>0.5374316931788463</v>
+        <v>0.5561841537769007</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
-        <is>
-          <t>Bynum, NC</t>
-        </is>
+      <c r="A44" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B44" t="n">
         <v>79.13583</v>
@@ -1790,29 +1704,27 @@
         <v>35.59861</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.04182154534098769</v>
+        <v>-0.0230358940087221</v>
       </c>
       <c r="E44" t="n">
-        <v>0.7951564233688819</v>
+        <v>0.8863225639572512</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.08483098543944284</v>
+        <v>-0.0830007167084286</v>
       </c>
       <c r="G44" t="n">
-        <v>0.5979593191737292</v>
+        <v>0.6059103641224776</v>
       </c>
       <c r="H44" t="n">
-        <v>0.06798240234922814</v>
+        <v>0.07067088453435834</v>
       </c>
       <c r="I44" t="n">
-        <v>0.6727862316575655</v>
+        <v>0.6606108179143221</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>Ramseur, NC</t>
-        </is>
+      <c r="A45" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B45" t="n">
         <v>79.65555999999999</v>
@@ -1821,29 +1733,27 @@
         <v>35.72639</v>
       </c>
       <c r="D45" t="n">
-        <v>0.08504982330491362</v>
+        <v>0.1135576964224642</v>
       </c>
       <c r="E45" t="n">
-        <v>0.5970117006627844</v>
+        <v>0.4796104282443501</v>
       </c>
       <c r="F45" t="n">
-        <v>0.02553365199940144</v>
+        <v>0.02437138881605128</v>
       </c>
       <c r="G45" t="n">
-        <v>0.8740906257184168</v>
+        <v>0.8797790017016476</v>
       </c>
       <c r="H45" t="n">
-        <v>0.07666230630200412</v>
+        <v>0.07314161252629725</v>
       </c>
       <c r="I45" t="n">
-        <v>0.6337895528486126</v>
+        <v>0.649497074786098</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="inlineStr">
-        <is>
-          <t>Moncure, NC</t>
-        </is>
+      <c r="A46" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B46" t="n">
         <v>79.11611000000001</v>
@@ -1852,29 +1762,27 @@
         <v>35.62694</v>
       </c>
       <c r="D46" t="n">
-        <v>-0.07668374742375664</v>
+        <v>-0.0585549693475801</v>
       </c>
       <c r="E46" t="n">
-        <v>0.6336943687683878</v>
+        <v>0.7161178589638948</v>
       </c>
       <c r="F46" t="n">
-        <v>-0.08876090215525249</v>
+        <v>-0.08562854852356422</v>
       </c>
       <c r="G46" t="n">
-        <v>0.5810429373380868</v>
+        <v>0.5945088567169249</v>
       </c>
       <c r="H46" t="n">
-        <v>0.08541705413791031</v>
+        <v>0.08933565264517536</v>
       </c>
       <c r="I46" t="n">
-        <v>0.5954229835043933</v>
+        <v>0.5785870747886835</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="inlineStr">
-        <is>
-          <t>Iverness, NC</t>
-        </is>
+      <c r="A47" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B47" t="n">
         <v>79.17749999999999</v>
@@ -1883,29 +1791,27 @@
         <v>35.18278</v>
       </c>
       <c r="D47" t="n">
-        <v>0.09451027070430712</v>
+        <v>0.1587756573699164</v>
       </c>
       <c r="E47" t="n">
-        <v>0.5566905011363421</v>
+        <v>0.321427931070528</v>
       </c>
       <c r="F47" t="n">
-        <v>-0.1603949596332495</v>
+        <v>-0.1622321939942829</v>
       </c>
       <c r="G47" t="n">
-        <v>0.3164534384219607</v>
+        <v>0.3108685849198893</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0511993653590451</v>
+        <v>0.05229216114246572</v>
       </c>
       <c r="I47" t="n">
-        <v>0.750556206454963</v>
+        <v>0.7454076565029568</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="inlineStr">
-        <is>
-          <t>Patterson, NC</t>
-        </is>
+      <c r="A48" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B48" t="n">
         <v>81.55833</v>
@@ -1914,29 +1820,27 @@
         <v>35.99083</v>
       </c>
       <c r="D48" t="n">
-        <v>0.234235847800449</v>
+        <v>0.2511955391808011</v>
       </c>
       <c r="E48" t="n">
-        <v>0.1404672494419234</v>
+        <v>0.11314484882612</v>
       </c>
       <c r="F48" t="n">
-        <v>0.1254863849649879</v>
+        <v>0.1257100013244147</v>
       </c>
       <c r="G48" t="n">
-        <v>0.4343592553868516</v>
+        <v>0.4335342831923318</v>
       </c>
       <c r="H48" t="n">
-        <v>0.2236904524104824</v>
+        <v>0.2165667622408414</v>
       </c>
       <c r="I48" t="n">
-        <v>0.1597506696888424</v>
+        <v>0.1738225060559506</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="inlineStr">
-        <is>
-          <t>Wilkesboro, NC</t>
-        </is>
+      <c r="A49" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B49" t="n">
         <v>81.16889</v>
@@ -1945,29 +1849,27 @@
         <v>36.175</v>
       </c>
       <c r="D49" t="n">
-        <v>0.2332163938932617</v>
+        <v>0.2601108894787701</v>
       </c>
       <c r="E49" t="n">
-        <v>0.14225253846014</v>
+        <v>0.1005020683420744</v>
       </c>
       <c r="F49" t="n">
-        <v>0.08336393216721552</v>
+        <v>0.08233525987770846</v>
       </c>
       <c r="G49" t="n">
-        <v>0.6043288720607737</v>
+        <v>0.6088124651479251</v>
       </c>
       <c r="H49" t="n">
-        <v>0.1845547801141302</v>
+        <v>0.1777271136052789</v>
       </c>
       <c r="I49" t="n">
-        <v>0.2480340429514857</v>
+        <v>0.2662695718419902</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="inlineStr">
-        <is>
-          <t>Wilkesboro, NC 1</t>
-        </is>
+      <c r="A50" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B50" t="n">
         <v>81.14556</v>
@@ -1976,29 +1878,27 @@
         <v>36.1525</v>
       </c>
       <c r="D50" t="n">
-        <v>0.2332163938932617</v>
+        <v>0.2601108894787701</v>
       </c>
       <c r="E50" t="n">
-        <v>0.14225253846014</v>
+        <v>0.1005020683420744</v>
       </c>
       <c r="F50" t="n">
-        <v>0.08336393216721552</v>
+        <v>0.08233525987770846</v>
       </c>
       <c r="G50" t="n">
-        <v>0.6043288720607737</v>
+        <v>0.6088124651479251</v>
       </c>
       <c r="H50" t="n">
-        <v>0.1845547801141302</v>
+        <v>0.1777271136052789</v>
       </c>
       <c r="I50" t="n">
-        <v>0.2480340429514857</v>
+        <v>0.2662695718419902</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="inlineStr">
-        <is>
-          <t>Elkin, NC</t>
-        </is>
+      <c r="A51" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B51" t="n">
         <v>80.84911</v>
@@ -2007,29 +1907,27 @@
         <v>36.24104</v>
       </c>
       <c r="D51" t="n">
-        <v>0.2769219379173602</v>
+        <v>0.3094987480893397</v>
       </c>
       <c r="E51" t="n">
-        <v>0.07963812449522908</v>
+        <v>0.04893935832495429</v>
       </c>
       <c r="F51" t="n">
-        <v>0.1418665072046215</v>
+        <v>0.1418430700192125</v>
       </c>
       <c r="G51" t="n">
-        <v>0.3762733884507722</v>
+        <v>0.376353053882399</v>
       </c>
       <c r="H51" t="n">
-        <v>0.1850523012526882</v>
+        <v>0.1772278411194974</v>
       </c>
       <c r="I51" t="n">
-        <v>0.2467389231941561</v>
+        <v>0.2676369351690476</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="inlineStr">
-        <is>
-          <t>Ararat, NC</t>
-        </is>
+      <c r="A52" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B52" t="n">
         <v>80.56169</v>
@@ -2038,29 +1936,27 @@
         <v>36.40439</v>
       </c>
       <c r="D52" t="n">
-        <v>0.1956842621711596</v>
+        <v>0.233375657718061</v>
       </c>
       <c r="E52" t="n">
-        <v>0.2201469340993439</v>
+        <v>0.1419725344510817</v>
       </c>
       <c r="F52" t="n">
-        <v>0.1025710883164949</v>
+        <v>0.102160507722982</v>
       </c>
       <c r="G52" t="n">
-        <v>0.5233754029027884</v>
+        <v>0.5250482330188101</v>
       </c>
       <c r="H52" t="n">
-        <v>0.1852332629660625</v>
+        <v>0.1785767780175311</v>
       </c>
       <c r="I52" t="n">
-        <v>0.2462689847219009</v>
+        <v>0.2639532244072839</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="inlineStr">
-        <is>
-          <t>Dalton, NC</t>
-        </is>
+      <c r="A53" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B53" t="n">
         <v>80.41472</v>
@@ -2069,29 +1965,27 @@
         <v>36.29917</v>
       </c>
       <c r="D53" t="n">
-        <v>0.09243395386615717</v>
+        <v>0.1207976456386131</v>
       </c>
       <c r="E53" t="n">
-        <v>0.5654297604966108</v>
+        <v>0.4518565427753407</v>
       </c>
       <c r="F53" t="n">
-        <v>-0.02663529573640311</v>
+        <v>-0.02275278127269881</v>
       </c>
       <c r="G53" t="n">
-        <v>0.8687046968961512</v>
+        <v>0.8877107117901966</v>
       </c>
       <c r="H53" t="n">
-        <v>0.1901078405780729</v>
+        <v>0.1919987761843933</v>
       </c>
       <c r="I53" t="n">
-        <v>0.2338366774823161</v>
+        <v>0.2291311134721544</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="inlineStr">
-        <is>
-          <t>Enon, NC</t>
-        </is>
+      <c r="A54" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B54" t="n">
         <v>80.44528</v>
@@ -2100,29 +1994,27 @@
         <v>36.13289</v>
       </c>
       <c r="D54" t="n">
-        <v>0.2203043685341526</v>
+        <v>0.2656182772068868</v>
       </c>
       <c r="E54" t="n">
-        <v>0.1663324379578029</v>
+        <v>0.09325112717398319</v>
       </c>
       <c r="F54" t="n">
-        <v>0.09348100344658113</v>
+        <v>0.09337513466154018</v>
       </c>
       <c r="G54" t="n">
-        <v>0.5610147945945456</v>
+        <v>0.5614604689649125</v>
       </c>
       <c r="H54" t="n">
-        <v>0.1627425734976388</v>
+        <v>0.1566203566631918</v>
       </c>
       <c r="I54" t="n">
-        <v>0.3093282872379806</v>
+        <v>0.3281246776939877</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="inlineStr">
-        <is>
-          <t>Mocksville, NC</t>
-        </is>
+      <c r="A55" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B55" t="n">
         <v>80.65889</v>
@@ -2131,29 +2023,27 @@
         <v>35.845</v>
       </c>
       <c r="D55" t="n">
-        <v>0.208740424037663</v>
+        <v>0.2461019015394585</v>
       </c>
       <c r="E55" t="n">
-        <v>0.1902841737941685</v>
+        <v>0.1208891483746145</v>
       </c>
       <c r="F55" t="n">
-        <v>0.09329486146428598</v>
+        <v>0.09318290432254761</v>
       </c>
       <c r="G55" t="n">
-        <v>0.5617985035832622</v>
+        <v>0.5622701187472012</v>
       </c>
       <c r="H55" t="n">
-        <v>0.06465704152556784</v>
+        <v>0.05999150517556973</v>
       </c>
       <c r="I55" t="n">
-        <v>0.6879604148016327</v>
+        <v>0.7094539859120639</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="inlineStr">
-        <is>
-          <t>Barber, NC</t>
-        </is>
+      <c r="A56" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B56" t="n">
         <v>80.59607</v>
@@ -2162,29 +2052,27 @@
         <v>35.71761</v>
       </c>
       <c r="D56" t="n">
-        <v>0.1565871921157592</v>
+        <v>0.1697898425050346</v>
       </c>
       <c r="E56" t="n">
-        <v>0.3282283979512274</v>
+        <v>0.2885565080910181</v>
       </c>
       <c r="F56" t="n">
-        <v>-0.01702251539384512</v>
+        <v>-0.01706198515625518</v>
       </c>
       <c r="G56" t="n">
-        <v>0.9158727065694732</v>
+        <v>0.9156783409746927</v>
       </c>
       <c r="H56" t="n">
-        <v>0.06173163107695448</v>
+        <v>0.06095962543551543</v>
       </c>
       <c r="I56" t="n">
-        <v>0.7014103624237505</v>
+        <v>0.7049750042169736</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>Norwood, NC</t>
-        </is>
+      <c r="A57" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B57" t="n">
         <v>80.16576999999999</v>
@@ -2193,29 +2081,27 @@
         <v>35.157</v>
       </c>
       <c r="D57" t="n">
-        <v>0.01456745933140486</v>
+        <v>0.007446483442747495</v>
       </c>
       <c r="E57" t="n">
-        <v>0.9279714828516245</v>
+        <v>0.9631454194156275</v>
       </c>
       <c r="F57" t="n">
-        <v>0.04932773229063706</v>
+        <v>0.05306453535852146</v>
       </c>
       <c r="G57" t="n">
-        <v>0.7593988717843173</v>
+        <v>0.7417752914906685</v>
       </c>
       <c r="H57" t="n">
-        <v>0.08220557197730352</v>
+        <v>0.08272939687946833</v>
       </c>
       <c r="I57" t="n">
-        <v>0.6093787341424465</v>
+        <v>0.6070928894753609</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="inlineStr">
-        <is>
-          <t>Rockingham, NC</t>
-        </is>
+      <c r="A58" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B58" t="n">
         <v>79.86972</v>
@@ -2224,29 +2110,27 @@
         <v>34.94583</v>
       </c>
       <c r="D58" t="n">
-        <v>0.07887529534456347</v>
+        <v>0.09985365239136122</v>
       </c>
       <c r="E58" t="n">
-        <v>0.6239963301900036</v>
+        <v>0.5344956890215625</v>
       </c>
       <c r="F58" t="n">
-        <v>0.03605850263372763</v>
+        <v>0.03792133245666931</v>
       </c>
       <c r="G58" t="n">
-        <v>0.8228977610023102</v>
+        <v>0.813905704961005</v>
       </c>
       <c r="H58" t="n">
-        <v>0.126766224752976</v>
+        <v>0.1251838062933175</v>
       </c>
       <c r="I58" t="n">
-        <v>0.4296494214380785</v>
+        <v>0.4354769237424302</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="inlineStr">
-        <is>
-          <t>Mcbee, SC</t>
-        </is>
+      <c r="A59" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B59" t="n">
         <v>80.18333</v>
@@ -2255,29 +2139,27 @@
         <v>34.51389</v>
       </c>
       <c r="D59" t="n">
-        <v>-0.01075059688830735</v>
+        <v>0.08866113235973921</v>
       </c>
       <c r="E59" t="n">
-        <v>0.9468122207130881</v>
+        <v>0.5814697226393079</v>
       </c>
       <c r="F59" t="n">
-        <v>-0.05659800669334329</v>
+        <v>-0.0530089349745798</v>
       </c>
       <c r="G59" t="n">
-        <v>0.7252293643816647</v>
+        <v>0.7420365886048897</v>
       </c>
       <c r="H59" t="n">
-        <v>0.07447090309984707</v>
+        <v>0.07764558033802191</v>
       </c>
       <c r="I59" t="n">
-        <v>0.643548382646741</v>
+        <v>0.6294304916844291</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="inlineStr">
-        <is>
-          <t>Hartsville, SC</t>
-        </is>
+      <c r="A60" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B60" t="n">
         <v>80.15000000000001</v>
@@ -2286,29 +2168,27 @@
         <v>32.39722</v>
       </c>
       <c r="D60" t="n">
-        <v>-0.09246972702563783</v>
+        <v>0.01490971874188952</v>
       </c>
       <c r="E60" t="n">
-        <v>0.5652786558990327</v>
+        <v>0.9262837699500691</v>
       </c>
       <c r="F60" t="n">
-        <v>-0.145056701251467</v>
+        <v>-0.1399670694651423</v>
       </c>
       <c r="G60" t="n">
-        <v>0.3655231079439821</v>
+        <v>0.3827621726105966</v>
       </c>
       <c r="H60" t="n">
-        <v>0.08699900715429251</v>
+        <v>0.09418665880709537</v>
       </c>
       <c r="I60" t="n">
-        <v>0.5886004217728861</v>
+        <v>0.5580484181631783</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="inlineStr">
-        <is>
-          <t>Effingham, SC</t>
-        </is>
+      <c r="A61" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B61" t="n">
         <v>79.75417</v>
@@ -2317,29 +2197,27 @@
         <v>34.05139</v>
       </c>
       <c r="D61" t="n">
-        <v>-0.02980978627681075</v>
+        <v>0.03718476493161631</v>
       </c>
       <c r="E61" t="n">
-        <v>0.8532181667874508</v>
+        <v>0.8174584375853523</v>
       </c>
       <c r="F61" t="n">
-        <v>-0.03684492018898661</v>
+        <v>-0.0345893467431964</v>
       </c>
       <c r="G61" t="n">
-        <v>0.8190988523873619</v>
+        <v>0.8300053735830958</v>
       </c>
       <c r="H61" t="n">
-        <v>0.0994515896475842</v>
+        <v>0.1009460534520035</v>
       </c>
       <c r="I61" t="n">
-        <v>0.536150683049687</v>
+        <v>0.530011632367235</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="inlineStr">
-        <is>
-          <t>Hoffman, NC</t>
-        </is>
+      <c r="A62" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B62" t="n">
         <v>79.49388999999999</v>
@@ -2348,29 +2226,27 @@
         <v>35.06111</v>
       </c>
       <c r="D62" t="n">
-        <v>-0.2171381751825434</v>
+        <v>-0.1436819506142313</v>
       </c>
       <c r="E62" t="n">
-        <v>0.1726620013145322</v>
+        <v>0.3701329344023743</v>
       </c>
       <c r="F62" t="n">
-        <v>-0.2559698075131664</v>
+        <v>-0.2509330659102606</v>
       </c>
       <c r="G62" t="n">
-        <v>0.1062327443394393</v>
+        <v>0.1135344954412591</v>
       </c>
       <c r="H62" t="n">
-        <v>0.1367059670076699</v>
+        <v>0.1468561951894296</v>
       </c>
       <c r="I62" t="n">
-        <v>0.3940550719143519</v>
+        <v>0.3595413475992715</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="inlineStr">
-        <is>
-          <t>Nebo, NC</t>
-        </is>
+      <c r="A63" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B63" t="n">
         <v>81.89111</v>
@@ -2379,29 +2255,27 @@
         <v>35.79556</v>
       </c>
       <c r="D63" t="n">
-        <v>0.2115753612344186</v>
+        <v>0.216096013543161</v>
       </c>
       <c r="E63" t="n">
-        <v>0.184198501332198</v>
+        <v>0.1747827658626709</v>
       </c>
       <c r="F63" t="n">
-        <v>0.0700864753485437</v>
+        <v>0.06659659667620499</v>
       </c>
       <c r="G63" t="n">
-        <v>0.6632502518463954</v>
+        <v>0.6790947646768425</v>
       </c>
       <c r="H63" t="n">
-        <v>0.2224100684683377</v>
+        <v>0.2141781747256834</v>
       </c>
       <c r="I63" t="n">
-        <v>0.1622168150088025</v>
+        <v>0.1787342083722269</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="inlineStr">
-        <is>
-          <t>Henry River, NC</t>
-        </is>
+      <c r="A64" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B64" t="n">
         <v>81.40333</v>
@@ -2410,29 +2284,27 @@
         <v>35.68444</v>
       </c>
       <c r="D64" t="n">
-        <v>0.1432532138238422</v>
+        <v>0.1825208738596802</v>
       </c>
       <c r="E64" t="n">
-        <v>0.3715776460857494</v>
+        <v>0.2533760838136769</v>
       </c>
       <c r="F64" t="n">
-        <v>0.01481485505107592</v>
+        <v>0.01971928101130657</v>
       </c>
       <c r="G64" t="n">
-        <v>0.9267515199936599</v>
+        <v>0.9026044116154482</v>
       </c>
       <c r="H64" t="n">
-        <v>0.1469754012436071</v>
+        <v>0.1477799344845557</v>
       </c>
       <c r="I64" t="n">
-        <v>0.3591471893897193</v>
+        <v>0.3564938066092221</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="inlineStr">
-        <is>
-          <t>Ramsey, NC</t>
-        </is>
+      <c r="A65" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B65" t="n">
         <v>81.56694</v>
@@ -2441,29 +2313,27 @@
         <v>35.59056</v>
       </c>
       <c r="D65" t="n">
-        <v>0.06669761690616603</v>
+        <v>0.1087831108884487</v>
       </c>
       <c r="E65" t="n">
-        <v>0.6786341583743976</v>
+        <v>0.4983906370964059</v>
       </c>
       <c r="F65" t="n">
-        <v>-0.01352486056697776</v>
+        <v>-0.00812650462446457</v>
       </c>
       <c r="G65" t="n">
-        <v>0.9331145228766774</v>
+        <v>0.9597824437622993</v>
       </c>
       <c r="H65" t="n">
-        <v>0.1491315794923248</v>
+        <v>0.1517464029529504</v>
       </c>
       <c r="I65" t="n">
-        <v>0.3520628386660713</v>
+        <v>0.3435865398256283</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="inlineStr">
-        <is>
-          <t>Laboratory, NC</t>
-        </is>
+      <c r="A66" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B66" t="n">
         <v>81.26528</v>
@@ -2472,29 +2342,27 @@
         <v>35.42056</v>
       </c>
       <c r="D66" t="n">
-        <v>0.05733335067803461</v>
+        <v>0.09441956394644292</v>
       </c>
       <c r="E66" t="n">
-        <v>0.7218011808628968</v>
+        <v>0.5570709621798854</v>
       </c>
       <c r="F66" t="n">
-        <v>-0.05309327113045466</v>
+        <v>-0.05021185001899088</v>
       </c>
       <c r="G66" t="n">
-        <v>0.7416402573331603</v>
+        <v>0.7552179496797267</v>
       </c>
       <c r="H66" t="n">
-        <v>0.181794077265503</v>
+        <v>0.1832884974809761</v>
       </c>
       <c r="I66" t="n">
-        <v>0.2553035402925303</v>
+        <v>0.2513509539321587</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="inlineStr">
-        <is>
-          <t>Bessemer City, NC</t>
-        </is>
+      <c r="A67" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B67" t="n">
         <v>81.23472</v>
@@ -2503,29 +2371,27 @@
         <v>35.30639</v>
       </c>
       <c r="D67" t="n">
-        <v>-0.02074955484557427</v>
+        <v>0.02874814726215072</v>
       </c>
       <c r="E67" t="n">
-        <v>0.8975420814173506</v>
+        <v>0.8583915460830787</v>
       </c>
       <c r="F67" t="n">
-        <v>-0.06349788966705092</v>
+        <v>-0.05878635326782203</v>
       </c>
       <c r="G67" t="n">
-        <v>0.6932786993475539</v>
+        <v>0.7150430838200302</v>
       </c>
       <c r="H67" t="n">
-        <v>0.1452883198592011</v>
+        <v>0.1494832787363322</v>
       </c>
       <c r="I67" t="n">
-        <v>0.3647498472062842</v>
+        <v>0.3509154146133219</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="inlineStr">
-        <is>
-          <t>Charlotte, NC</t>
-        </is>
+      <c r="A68" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B68" t="n">
         <v>80.85778000000001</v>
@@ -2534,29 +2400,27 @@
         <v>35.14806</v>
       </c>
       <c r="D68" t="n">
-        <v>0.1076313015102054</v>
+        <v>0.1171015510164877</v>
       </c>
       <c r="E68" t="n">
-        <v>0.5029766998498251</v>
+        <v>0.4659149410206934</v>
       </c>
       <c r="F68" t="n">
-        <v>0.1264526262982867</v>
+        <v>0.1246186803111257</v>
       </c>
       <c r="G68" t="n">
-        <v>0.4308008245962829</v>
+        <v>0.437568655477946</v>
       </c>
       <c r="H68" t="n">
-        <v>0.03366007956291526</v>
+        <v>0.02805354610204237</v>
       </c>
       <c r="I68" t="n">
-        <v>0.8345080137373206</v>
+        <v>0.8617795246576591</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="inlineStr">
-        <is>
-          <t>Charlotte, NC 1</t>
-        </is>
+      <c r="A69" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B69" t="n">
         <v>80.7675</v>
@@ -2565,29 +2429,27 @@
         <v>35.13778</v>
       </c>
       <c r="D69" t="n">
-        <v>0.1353653917478582</v>
+        <v>0.1197538915944799</v>
       </c>
       <c r="E69" t="n">
-        <v>0.398752968231646</v>
+        <v>0.455803016661557</v>
       </c>
       <c r="F69" t="n">
-        <v>0.09292383282198959</v>
+        <v>0.09349974207792811</v>
       </c>
       <c r="G69" t="n">
-        <v>0.5633621515220865</v>
+        <v>0.5609359279776568</v>
       </c>
       <c r="H69" t="n">
-        <v>0.09479956275522818</v>
+        <v>0.09137086519387755</v>
       </c>
       <c r="I69" t="n">
-        <v>0.5554779063060776</v>
+        <v>0.5699286996344761</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="inlineStr">
-        <is>
-          <t>Lake Lure, NC</t>
-        </is>
+      <c r="A70" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B70" t="n">
         <v>82.11167</v>
@@ -2596,29 +2458,27 @@
         <v>35.42333</v>
       </c>
       <c r="D70" t="n">
-        <v>0.1029368483115611</v>
+        <v>0.1251701391542882</v>
       </c>
       <c r="E70" t="n">
-        <v>0.5218874022427337</v>
+        <v>0.4355274451699799</v>
       </c>
       <c r="F70" t="n">
-        <v>0.01049810736186942</v>
+        <v>0.008985008045014901</v>
       </c>
       <c r="G70" t="n">
-        <v>0.9480596763265815</v>
+        <v>0.9555377914945437</v>
       </c>
       <c r="H70" t="n">
-        <v>0.1232543250996237</v>
+        <v>0.1191244896415139</v>
       </c>
       <c r="I70" t="n">
-        <v>0.4426414444394809</v>
+        <v>0.4581917853075314</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="inlineStr">
-        <is>
-          <t>Boiling Springs, NC</t>
-        </is>
+      <c r="A71" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B71" t="n">
         <v>81.69750000000001</v>
@@ -2627,29 +2487,27 @@
         <v>35.21083</v>
       </c>
       <c r="D71" t="n">
-        <v>0.05334785802934139</v>
+        <v>0.1037178791511</v>
       </c>
       <c r="E71" t="n">
-        <v>0.7404442455630381</v>
+        <v>0.5187169930706462</v>
       </c>
       <c r="F71" t="n">
-        <v>-0.03239174427407712</v>
+        <v>-0.0332205624294122</v>
       </c>
       <c r="G71" t="n">
-        <v>0.8406619603971381</v>
+        <v>0.8366394621539041</v>
       </c>
       <c r="H71" t="n">
-        <v>0.1029715413325374</v>
+        <v>0.1008522212795031</v>
       </c>
       <c r="I71" t="n">
-        <v>0.5217463712272695</v>
+        <v>0.5303960696468475</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="inlineStr">
-        <is>
-          <t>Casar, NC</t>
-        </is>
+      <c r="A72" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B72" t="n">
         <v>81.68222</v>
@@ -2658,29 +2516,27 @@
         <v>35.49306</v>
       </c>
       <c r="D72" t="n">
-        <v>0.1194760311764377</v>
+        <v>0.1573471093846242</v>
       </c>
       <c r="E72" t="n">
-        <v>0.4568567489921556</v>
+        <v>0.3258569301763958</v>
       </c>
       <c r="F72" t="n">
-        <v>0.08084910683045907</v>
+        <v>0.08438929667741678</v>
       </c>
       <c r="G72" t="n">
-        <v>0.6153150299329262</v>
+        <v>0.5998739299425119</v>
       </c>
       <c r="H72" t="n">
-        <v>0.1338952759092111</v>
+        <v>0.1318993330993728</v>
       </c>
       <c r="I72" t="n">
-        <v>0.4039418865698325</v>
+        <v>0.4110485507404095</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="inlineStr">
-        <is>
-          <t>Fingerville, SC</t>
-        </is>
+      <c r="A73" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B73" t="n">
         <v>81.98611</v>
@@ -2689,29 +2545,27 @@
         <v>35.12083</v>
       </c>
       <c r="D73" t="n">
-        <v>0.04860985826550886</v>
+        <v>0.08769852657826183</v>
       </c>
       <c r="E73" t="n">
-        <v>0.7627986248149758</v>
+        <v>0.5855946782118754</v>
       </c>
       <c r="F73" t="n">
-        <v>-0.02641432027254487</v>
+        <v>-0.02561815932830582</v>
       </c>
       <c r="G73" t="n">
-        <v>0.8697845831271618</v>
+        <v>0.8736772682084455</v>
       </c>
       <c r="H73" t="n">
-        <v>0.1314110067659036</v>
+        <v>0.1303406201317298</v>
       </c>
       <c r="I73" t="n">
-        <v>0.4127980590373493</v>
+        <v>0.416647689205974</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="inlineStr">
-        <is>
-          <t>Carlisle, SC</t>
-        </is>
+      <c r="A74" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B74" t="n">
         <v>81.42139</v>
@@ -2720,29 +2574,27 @@
         <v>34.595</v>
       </c>
       <c r="D74" t="n">
-        <v>0.03178461444994388</v>
+        <v>0.08353783865002889</v>
       </c>
       <c r="E74" t="n">
-        <v>0.8436110849761278</v>
+        <v>0.60357228928258</v>
       </c>
       <c r="F74" t="n">
-        <v>-0.05996910150835362</v>
+        <v>-0.05688794813551992</v>
       </c>
       <c r="G74" t="n">
-        <v>0.7095577508661484</v>
+        <v>0.7238770171956036</v>
       </c>
       <c r="H74" t="n">
-        <v>0.1463731210121639</v>
+        <v>0.14820551146827</v>
       </c>
       <c r="I74" t="n">
-        <v>0.3611413177548002</v>
+        <v>0.355095050611281</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="inlineStr">
-        <is>
-          <t>Delta, SC</t>
-        </is>
+      <c r="A75" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B75" t="n">
         <v>81.54833000000001</v>
@@ -2751,29 +2603,27 @@
         <v>34.53528</v>
       </c>
       <c r="D75" t="n">
-        <v>-0.09356540930788911</v>
+        <v>-0.01053710498979998</v>
       </c>
       <c r="E75" t="n">
-        <v>0.5606595903247455</v>
+        <v>0.9478669956772828</v>
       </c>
       <c r="F75" t="n">
-        <v>-0.1249484718684174</v>
+        <v>-0.1190024119865923</v>
       </c>
       <c r="G75" t="n">
-        <v>0.4363473055956893</v>
+        <v>0.4586558865200402</v>
       </c>
       <c r="H75" t="n">
-        <v>0.1542375788611091</v>
+        <v>0.1607680351854529</v>
       </c>
       <c r="I75" t="n">
-        <v>0.3356286507976939</v>
+        <v>0.3153142702304209</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="inlineStr">
-        <is>
-          <t>Whitmire, SC</t>
-        </is>
+      <c r="A76" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B76" t="n">
         <v>81.59833</v>
@@ -2782,29 +2632,27 @@
         <v>34.50917</v>
       </c>
       <c r="D76" t="n">
-        <v>0.00812566672829609</v>
+        <v>0.07178243861393802</v>
       </c>
       <c r="E76" t="n">
-        <v>0.959786587081351</v>
+        <v>0.6556017809290211</v>
       </c>
       <c r="F76" t="n">
-        <v>-0.008473311722637919</v>
+        <v>-0.005423339562119628</v>
       </c>
       <c r="G76" t="n">
-        <v>0.9580676056456674</v>
+        <v>0.973154174587802</v>
       </c>
       <c r="H76" t="n">
-        <v>0.1194449671902817</v>
+        <v>0.1200587920669505</v>
       </c>
       <c r="I76" t="n">
-        <v>0.4569746348825524</v>
+        <v>0.4546482537829559</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="inlineStr">
-        <is>
-          <t>Ware Shoals, SC</t>
-        </is>
+      <c r="A77" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B77" t="n">
         <v>82.22360999999999</v>
@@ -2813,29 +2661,27 @@
         <v>34.39167</v>
       </c>
       <c r="D77" t="n">
-        <v>0.07476944848136149</v>
+        <v>0.1284019945531452</v>
       </c>
       <c r="E77" t="n">
-        <v>0.6422153620916126</v>
+        <v>0.4236714798816155</v>
       </c>
       <c r="F77" t="n">
-        <v>0.03352754378599788</v>
+        <v>0.03458763283632872</v>
       </c>
       <c r="G77" t="n">
-        <v>0.8351506267240398</v>
+        <v>0.8300136732005295</v>
       </c>
       <c r="H77" t="n">
-        <v>0.1336099855550432</v>
+        <v>0.1312330926392812</v>
       </c>
       <c r="I77" t="n">
-        <v>0.4049533266842229</v>
+        <v>0.4134365173909552</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>Chappels, SC</t>
-        </is>
+      <c r="A78" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B78" t="n">
         <v>81.86417</v>
@@ -2844,29 +2690,27 @@
         <v>34.17444</v>
       </c>
       <c r="D78" t="n">
-        <v>0.09980316705186242</v>
+        <v>0.1654967693766706</v>
       </c>
       <c r="E78" t="n">
-        <v>0.5347033636197456</v>
+        <v>0.3011000756836239</v>
       </c>
       <c r="F78" t="n">
-        <v>0.05850642658047595</v>
+        <v>0.05989585083040522</v>
       </c>
       <c r="G78" t="n">
-        <v>0.716343408141932</v>
+        <v>0.7098970552535624</v>
       </c>
       <c r="H78" t="n">
-        <v>0.1465277702680186</v>
+        <v>0.1435253985435408</v>
       </c>
       <c r="I78" t="n">
-        <v>0.3606286440200108</v>
+        <v>0.3706600778143507</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="inlineStr">
-        <is>
-          <t>Clayton, GA</t>
-        </is>
+      <c r="A79" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B79" t="n">
         <v>83.30611</v>
@@ -2875,29 +2719,27 @@
         <v>34.81389</v>
       </c>
       <c r="D79" t="n">
-        <v>0.08751581516893783</v>
+        <v>0.124195883544852</v>
       </c>
       <c r="E79" t="n">
-        <v>0.5863791042598037</v>
+        <v>0.4391372021996756</v>
       </c>
       <c r="F79" t="n">
-        <v>0.02540678147019199</v>
+        <v>0.0209667052336472</v>
       </c>
       <c r="G79" t="n">
-        <v>0.8747112597378709</v>
+        <v>0.8964756005483588</v>
       </c>
       <c r="H79" t="n">
-        <v>0.2100361291089686</v>
+        <v>0.2031510721975528</v>
       </c>
       <c r="I79" t="n">
-        <v>0.1874853073222449</v>
+        <v>0.2026965291913578</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="inlineStr">
-        <is>
-          <t>Clayton, GA 1</t>
-        </is>
+      <c r="A80" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B80" t="n">
         <v>83.53064000000001</v>
@@ -2906,29 +2748,27 @@
         <v>34.88997</v>
       </c>
       <c r="D80" t="n">
-        <v>0.1311095714426093</v>
+        <v>0.1521181244780143</v>
       </c>
       <c r="E80" t="n">
-        <v>0.4138801128264526</v>
+        <v>0.3423918095428941</v>
       </c>
       <c r="F80" t="n">
-        <v>0.03146452825593015</v>
+        <v>0.02605275855981547</v>
       </c>
       <c r="G80" t="n">
-        <v>0.8451667504971578</v>
+        <v>0.8715520035991726</v>
       </c>
       <c r="H80" t="n">
-        <v>0.2570469769000913</v>
+        <v>0.2487574262795003</v>
       </c>
       <c r="I80" t="n">
-        <v>0.1047186914656979</v>
+        <v>0.1168034711677</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="inlineStr">
-        <is>
-          <t>Cornelia, GA</t>
-        </is>
+      <c r="A81" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B81" t="n">
         <v>83.62277</v>
@@ -2937,29 +2777,27 @@
         <v>34.54072</v>
       </c>
       <c r="D81" t="n">
-        <v>-0.009448755797855951</v>
+        <v>0.04728997317738823</v>
       </c>
       <c r="E81" t="n">
-        <v>0.9532454049915883</v>
+        <v>0.7690608654462892</v>
       </c>
       <c r="F81" t="n">
-        <v>-0.06823125143730349</v>
+        <v>-0.0704023426121289</v>
       </c>
       <c r="G81" t="n">
-        <v>0.6716557332900503</v>
+        <v>0.6618231631334618</v>
       </c>
       <c r="H81" t="n">
-        <v>0.2464835141349001</v>
+        <v>0.2440071528399335</v>
       </c>
       <c r="I81" t="n">
-        <v>0.1202954951561785</v>
+        <v>0.1241871261643465</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="inlineStr">
-        <is>
-          <t>Jefferson, NC</t>
-        </is>
+      <c r="A82" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B82" t="n">
         <v>81.40694000000001</v>
@@ -2968,29 +2806,27 @@
         <v>36.39333</v>
       </c>
       <c r="D82" t="n">
-        <v>0.3173036745970545</v>
+        <v>0.3298594461943306</v>
       </c>
       <c r="E82" t="n">
-        <v>0.043230583015778</v>
+        <v>0.03519031888076782</v>
       </c>
       <c r="F82" t="n">
-        <v>0.1453874087676685</v>
+        <v>0.1415328401151434</v>
       </c>
       <c r="G82" t="n">
-        <v>0.3644193382024701</v>
+        <v>0.3774084997372285</v>
       </c>
       <c r="H82" t="n">
-        <v>0.2438405637864977</v>
+        <v>0.2323929630919202</v>
       </c>
       <c r="I82" t="n">
-        <v>0.1244522708023712</v>
+        <v>0.1437067258853273</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>Galax, VA</t>
-        </is>
+      <c r="A83" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B83" t="n">
         <v>80.97917</v>
@@ -2999,29 +2835,27 @@
         <v>36.64722</v>
       </c>
       <c r="D83" t="n">
-        <v>0.3167218417952631</v>
+        <v>0.3245073008220288</v>
       </c>
       <c r="E83" t="n">
-        <v>0.04363659165110449</v>
+        <v>0.03845316614947258</v>
       </c>
       <c r="F83" t="n">
-        <v>0.1461507931447742</v>
+        <v>0.1438831723311569</v>
       </c>
       <c r="G83" t="n">
-        <v>0.3618791202487607</v>
+        <v>0.3694560366717436</v>
       </c>
       <c r="H83" t="n">
-        <v>0.2633571434718229</v>
+        <v>0.2529709152102273</v>
       </c>
       <c r="I83" t="n">
-        <v>0.09617767145176512</v>
+        <v>0.1105358019120727</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="inlineStr">
-        <is>
-          <t>Allisonia, VA</t>
-        </is>
+      <c r="A84" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B84" t="n">
         <v>80.74583</v>
@@ -3030,29 +2864,27 @@
         <v>36.9375</v>
       </c>
       <c r="D84" t="n">
-        <v>0.3174334916511521</v>
+        <v>0.3283262187783292</v>
       </c>
       <c r="E84" t="n">
-        <v>0.04314041518161867</v>
+        <v>0.03610092250666532</v>
       </c>
       <c r="F84" t="n">
-        <v>0.1573031429738787</v>
+        <v>0.1558902136802628</v>
       </c>
       <c r="G84" t="n">
-        <v>0.325993843318426</v>
+        <v>0.3304128848180686</v>
       </c>
       <c r="H84" t="n">
-        <v>0.2562915113685438</v>
+        <v>0.246316863735892</v>
       </c>
       <c r="I84" t="n">
-        <v>0.1057788263518227</v>
+        <v>0.1205544734851556</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="inlineStr">
-        <is>
-          <t>Graysontown, VA</t>
-        </is>
+      <c r="A85" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B85" t="n">
         <v>80.55694</v>
@@ -3061,29 +2893,27 @@
         <v>37.0375</v>
       </c>
       <c r="D85" t="n">
-        <v>0.3449258272701706</v>
+        <v>0.3835796410126046</v>
       </c>
       <c r="E85" t="n">
-        <v>0.02720434898979865</v>
+        <v>0.01329876640036455</v>
       </c>
       <c r="F85" t="n">
-        <v>0.1452648555172571</v>
+        <v>0.1412153247099693</v>
       </c>
       <c r="G85" t="n">
-        <v>0.3648281383781757</v>
+        <v>0.3784905452167987</v>
       </c>
       <c r="H85" t="n">
-        <v>0.1625248177611847</v>
+        <v>0.1512466672592009</v>
       </c>
       <c r="I85" t="n">
-        <v>0.3099848684992481</v>
+        <v>0.345196739740339</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="inlineStr">
-        <is>
-          <t>Radford, VA</t>
-        </is>
+      <c r="A86" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B86" t="n">
         <v>80.56944</v>
@@ -3092,29 +2922,27 @@
         <v>37.14167</v>
       </c>
       <c r="D86" t="n">
-        <v>0.3291896145076201</v>
+        <v>0.3541287929848147</v>
       </c>
       <c r="E86" t="n">
-        <v>0.03558579622028373</v>
+        <v>0.023112069424777</v>
       </c>
       <c r="F86" t="n">
-        <v>0.1603237587060067</v>
+        <v>0.1583675112033303</v>
       </c>
       <c r="G86" t="n">
-        <v>0.3166711415440695</v>
+        <v>0.3226894544700284</v>
       </c>
       <c r="H86" t="n">
-        <v>0.2476704931965832</v>
+        <v>0.2371445422801307</v>
       </c>
       <c r="I86" t="n">
-        <v>0.1184629951885616</v>
+        <v>0.1354645400933361</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="inlineStr">
-        <is>
-          <t>Bane, VA</t>
-        </is>
+      <c r="A87" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B87" t="n">
         <v>80.70972</v>
@@ -3123,29 +2951,27 @@
         <v>37.26806</v>
       </c>
       <c r="D87" t="n">
-        <v>0.336568040618861</v>
+        <v>0.3556203828065471</v>
       </c>
       <c r="E87" t="n">
-        <v>0.03142472628875204</v>
+        <v>0.02249986692880758</v>
       </c>
       <c r="F87" t="n">
-        <v>0.1189307668644806</v>
+        <v>0.1164303689096666</v>
       </c>
       <c r="G87" t="n">
-        <v>0.4589283768273595</v>
+        <v>0.4684926347774552</v>
       </c>
       <c r="H87" t="n">
-        <v>0.2021490191200331</v>
+        <v>0.1929431141690877</v>
       </c>
       <c r="I87" t="n">
-        <v>0.2049803517269821</v>
+        <v>0.2268055578786665</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="inlineStr">
-        <is>
-          <t>Glen Lyn, VA</t>
-        </is>
+      <c r="A88" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B88" t="n">
         <v>80.86083000000001</v>
@@ -3154,29 +2980,27 @@
         <v>37.37278</v>
       </c>
       <c r="D88" t="n">
-        <v>0.3032296730123487</v>
+        <v>0.3312940571280412</v>
       </c>
       <c r="E88" t="n">
-        <v>0.05395227079658037</v>
+        <v>0.03435542492295347</v>
       </c>
       <c r="F88" t="n">
-        <v>0.1537228293419327</v>
+        <v>0.1519073733423481</v>
       </c>
       <c r="G88" t="n">
-        <v>0.337263561385343</v>
+        <v>0.3430688597921543</v>
       </c>
       <c r="H88" t="n">
-        <v>0.2344951594977058</v>
+        <v>0.2245295158191377</v>
       </c>
       <c r="I88" t="n">
-        <v>0.1400157903928841</v>
+        <v>0.1581493977194391</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1" t="inlineStr">
-        <is>
-          <t>Durbin, WV</t>
-        </is>
+      <c r="A89" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B89" t="n">
         <v>79.83333</v>
@@ -3185,29 +3009,27 @@
         <v>38.54361</v>
       </c>
       <c r="D89" t="n">
-        <v>-0.1727297824105222</v>
+        <v>-0.09567191635678664</v>
       </c>
       <c r="E89" t="n">
-        <v>0.2801647511424584</v>
+        <v>0.5518288777955691</v>
       </c>
       <c r="F89" t="n">
-        <v>-0.2690267620832386</v>
+        <v>-0.2753266185904495</v>
       </c>
       <c r="G89" t="n">
-        <v>0.08896994012010496</v>
+        <v>0.08145926733847006</v>
       </c>
       <c r="H89" t="n">
-        <v>0.3403354841990687</v>
+        <v>0.3394145958927542</v>
       </c>
       <c r="I89" t="n">
-        <v>0.02945995590914945</v>
+        <v>0.02993057693490473</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="1" t="inlineStr">
-        <is>
-          <t>Buckeye, WV</t>
-        </is>
+      <c r="A90" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B90" t="n">
         <v>80.13</v>
@@ -3216,29 +3038,27 @@
         <v>38.18622</v>
       </c>
       <c r="D90" t="n">
-        <v>-0.1224282102102457</v>
+        <v>-0.003794143540432504</v>
       </c>
       <c r="E90" t="n">
-        <v>0.4457286480347842</v>
+        <v>0.9812170442313206</v>
       </c>
       <c r="F90" t="n">
-        <v>-0.282940268306441</v>
+        <v>-0.288133061552082</v>
       </c>
       <c r="G90" t="n">
-        <v>0.07305262574302819</v>
+        <v>0.06772145199819214</v>
       </c>
       <c r="H90" t="n">
-        <v>0.2911863747171883</v>
+        <v>0.2914185387303232</v>
       </c>
       <c r="I90" t="n">
-        <v>0.06473335763719502</v>
+        <v>0.06451049952067558</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="inlineStr">
-        <is>
-          <t>Alderson, WV</t>
-        </is>
+      <c r="A91" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B91" t="n">
         <v>80.64167</v>
@@ -3247,29 +3067,27 @@
         <v>37.72417</v>
       </c>
       <c r="D91" t="n">
-        <v>-0.03343371341767709</v>
+        <v>0.1010968034217832</v>
       </c>
       <c r="E91" t="n">
-        <v>0.8356056366389775</v>
+        <v>0.5293942837025546</v>
       </c>
       <c r="F91" t="n">
-        <v>-0.1735966861341853</v>
+        <v>-0.1775754068097196</v>
       </c>
       <c r="G91" t="n">
-        <v>0.2777210011123402</v>
+        <v>0.2666845634525232</v>
       </c>
       <c r="H91" t="n">
-        <v>0.2638847519073276</v>
+        <v>0.2613764458449779</v>
       </c>
       <c r="I91" t="n">
-        <v>0.09548856189825422</v>
+        <v>0.09879882690744246</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="inlineStr">
-        <is>
-          <t>Hilldale, WV</t>
-        </is>
+      <c r="A92" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B92" t="n">
         <v>80.80528</v>
@@ -3278,29 +3096,27 @@
         <v>37.64</v>
       </c>
       <c r="D92" t="n">
-        <v>-0.004417977638052323</v>
+        <v>0.1234985030569003</v>
       </c>
       <c r="E92" t="n">
-        <v>0.9781294365021411</v>
+        <v>0.44173120312436</v>
       </c>
       <c r="F92" t="n">
-        <v>-0.1587357347111657</v>
+        <v>-0.1625078301930074</v>
       </c>
       <c r="G92" t="n">
-        <v>0.32155118975612</v>
+        <v>0.310036126898507</v>
       </c>
       <c r="H92" t="n">
-        <v>0.2698281044756683</v>
+        <v>0.2669344990270794</v>
       </c>
       <c r="I92" t="n">
-        <v>0.08798587102873537</v>
+        <v>0.09157946514207324</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="inlineStr">
-        <is>
-          <t>Dyer, WV</t>
-        </is>
+      <c r="A93" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B93" t="n">
         <v>80.48417000000001</v>
@@ -3309,29 +3125,27 @@
         <v>38.37889</v>
       </c>
       <c r="D93" t="n">
-        <v>-0.1365989759774304</v>
+        <v>-0.02672583446902329</v>
       </c>
       <c r="E93" t="n">
-        <v>0.3944288235356874</v>
+        <v>0.8682623105061699</v>
       </c>
       <c r="F93" t="n">
-        <v>-0.2982373012864021</v>
+        <v>-0.3006127364576704</v>
       </c>
       <c r="G93" t="n">
-        <v>0.05823199327394664</v>
+        <v>0.05616304202181677</v>
       </c>
       <c r="H93" t="n">
-        <v>0.2782971717970906</v>
+        <v>0.2816848061779803</v>
       </c>
       <c r="I93" t="n">
-        <v>0.07809388164823651</v>
+        <v>0.07438979309760532</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="inlineStr">
-        <is>
-          <t>Belva, WV</t>
-        </is>
+      <c r="A94" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B94" t="n">
         <v>81.18111</v>
@@ -3340,29 +3154,27 @@
         <v>38.23333</v>
       </c>
       <c r="D94" t="n">
-        <v>0.06855462245085306</v>
+        <v>0.19013106965518</v>
       </c>
       <c r="E94" t="n">
-        <v>0.6701877547577152</v>
+        <v>0.2337784760292522</v>
       </c>
       <c r="F94" t="n">
-        <v>-0.1292448192992319</v>
+        <v>-0.1309783395648082</v>
       </c>
       <c r="G94" t="n">
-        <v>0.4206097167206681</v>
+        <v>0.4143516956359942</v>
       </c>
       <c r="H94" t="n">
-        <v>0.3291922238326291</v>
+        <v>0.3269395594102448</v>
       </c>
       <c r="I94" t="n">
-        <v>0.0355842486034935</v>
+        <v>0.03694101235197052</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="1" t="inlineStr">
-        <is>
-          <t>Kanawha Falls, WV</t>
-        </is>
+      <c r="A95" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B95" t="n">
         <v>81.21444</v>
@@ -3371,29 +3183,27 @@
         <v>39.13806</v>
       </c>
       <c r="D95" t="n">
-        <v>0.2117639138613956</v>
+        <v>0.2989358093185399</v>
       </c>
       <c r="E95" t="n">
-        <v>0.1837987110844902</v>
+        <v>0.05761739223545697</v>
       </c>
       <c r="F95" t="n">
-        <v>0.01025991992053722</v>
+        <v>0.007946609144926814</v>
       </c>
       <c r="G95" t="n">
-        <v>0.9492365829398673</v>
+        <v>0.9606720340403143</v>
       </c>
       <c r="H95" t="n">
-        <v>0.3282926596287413</v>
+        <v>0.3210358453944907</v>
       </c>
       <c r="I95" t="n">
-        <v>0.03612106749433364</v>
+        <v>0.04069859129728375</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="inlineStr">
-        <is>
-          <t>Queen Shoals, WV</t>
-        </is>
+      <c r="A96" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B96" t="n">
         <v>81.28417</v>
@@ -3402,29 +3212,27 @@
         <v>38.6375</v>
       </c>
       <c r="D96" t="n">
-        <v>0.1195233449614561</v>
+        <v>0.203529058888487</v>
       </c>
       <c r="E96" t="n">
-        <v>0.4566772276828667</v>
+        <v>0.2018396880268656</v>
       </c>
       <c r="F96" t="n">
-        <v>-0.1879424254382801</v>
+        <v>-0.1919315001048135</v>
       </c>
       <c r="G96" t="n">
-        <v>0.239305600586368</v>
+        <v>0.2292974095358573</v>
       </c>
       <c r="H96" t="n">
-        <v>0.3926468156584685</v>
+        <v>0.3895218919071449</v>
       </c>
       <c r="I96" t="n">
-        <v>0.0111071060659898</v>
+        <v>0.01182476038702629</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="inlineStr">
-        <is>
-          <t>Ashford, WV</t>
-        </is>
+      <c r="A97" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B97" t="n">
         <v>81.71167</v>
@@ -3433,29 +3241,27 @@
         <v>38.17972</v>
       </c>
       <c r="D97" t="n">
-        <v>0.1572783280788429</v>
+        <v>0.210286449771157</v>
       </c>
       <c r="E97" t="n">
-        <v>0.3260711337450012</v>
+        <v>0.1869479707726239</v>
       </c>
       <c r="F97" t="n">
-        <v>0.07466622338539887</v>
+        <v>0.07495967078032847</v>
       </c>
       <c r="G97" t="n">
-        <v>0.6426761424865276</v>
+        <v>0.6413665866925586</v>
       </c>
       <c r="H97" t="n">
-        <v>0.2583623612158554</v>
+        <v>0.2533435563092689</v>
       </c>
       <c r="I97" t="n">
-        <v>0.1028921977770593</v>
+        <v>0.1099940226446683</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="inlineStr">
-        <is>
-          <t>Tornado, WV</t>
-        </is>
+      <c r="A98" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B98" t="n">
         <v>81.84166999999999</v>
@@ -3464,29 +3270,27 @@
         <v>38.33889</v>
       </c>
       <c r="D98" t="n">
-        <v>0.2319156253027969</v>
+        <v>0.2847335401571236</v>
       </c>
       <c r="E98" t="n">
-        <v>0.1445547090326048</v>
+        <v>0.0711755021085777</v>
       </c>
       <c r="F98" t="n">
-        <v>0.108030971963038</v>
+        <v>0.1068326316930253</v>
       </c>
       <c r="G98" t="n">
-        <v>0.5013829419282895</v>
+        <v>0.5061692286152293</v>
       </c>
       <c r="H98" t="n">
-        <v>0.2709709838584657</v>
+        <v>0.263417385047312</v>
       </c>
       <c r="I98" t="n">
-        <v>0.08659700239520478</v>
+        <v>0.09609879709345076</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="inlineStr">
-        <is>
-          <t>Baileysville, WV</t>
-        </is>
+      <c r="A99" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B99" t="n">
         <v>81.64528</v>
@@ -3495,29 +3299,27 @@
         <v>37.60389</v>
       </c>
       <c r="D99" t="n">
-        <v>0.2319156253027969</v>
+        <v>0.2847335401571236</v>
       </c>
       <c r="E99" t="n">
-        <v>0.1445547090326048</v>
+        <v>0.0711755021085777</v>
       </c>
       <c r="F99" t="n">
-        <v>0.108030971963038</v>
+        <v>0.1068326316930253</v>
       </c>
       <c r="G99" t="n">
-        <v>0.5013829419282895</v>
+        <v>0.5061692286152293</v>
       </c>
       <c r="H99" t="n">
-        <v>0.2709709838584657</v>
+        <v>0.263417385047312</v>
       </c>
       <c r="I99" t="n">
-        <v>0.08659700239520478</v>
+        <v>0.09609879709345076</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="inlineStr">
-        <is>
-          <t>Clear Fork, WV</t>
-        </is>
+      <c r="A100" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B100" t="n">
         <v>81.7075</v>
@@ -3526,29 +3328,27 @@
         <v>37.62306</v>
       </c>
       <c r="D100" t="n">
-        <v>0.06478061652527464</v>
+        <v>0.1756837495698607</v>
       </c>
       <c r="E100" t="n">
-        <v>0.6873943108780911</v>
+        <v>0.2718950636950987</v>
       </c>
       <c r="F100" t="n">
-        <v>0.09923683193239213</v>
+        <v>0.0995891273481604</v>
       </c>
       <c r="G100" t="n">
-        <v>0.5370356956424891</v>
+        <v>0.535584263553468</v>
       </c>
       <c r="H100" t="n">
-        <v>0.2503382923236278</v>
+        <v>0.2452519039414632</v>
       </c>
       <c r="I100" t="n">
-        <v>0.1144212052695687</v>
+        <v>0.1222193552904196</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="1" t="inlineStr">
-        <is>
-          <t>Logan, WV</t>
-        </is>
+      <c r="A101" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B101" t="n">
         <v>81.97611000000001</v>
@@ -3557,29 +3357,27 @@
         <v>37.84222</v>
       </c>
       <c r="D101" t="n">
-        <v>0.07520404023316016</v>
+        <v>0.1718123416376657</v>
       </c>
       <c r="E101" t="n">
-        <v>0.6402768665037836</v>
+        <v>0.2827662054123329</v>
       </c>
       <c r="F101" t="n">
-        <v>0.113920699034494</v>
+        <v>0.112382038939236</v>
       </c>
       <c r="G101" t="n">
-        <v>0.4781979499197086</v>
+        <v>0.4841999977478537</v>
       </c>
       <c r="H101" t="n">
-        <v>0.2196664256686992</v>
+        <v>0.2129383847252305</v>
       </c>
       <c r="I101" t="n">
-        <v>0.1675940679461244</v>
+        <v>0.1813223644050501</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="inlineStr">
-        <is>
-          <t>Big Rock, VA</t>
-        </is>
+      <c r="A102" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B102" t="n">
         <v>82.19583</v>
@@ -3588,29 +3386,27 @@
         <v>37.35361</v>
       </c>
       <c r="D102" t="n">
-        <v>0.2924522485218396</v>
+        <v>0.409605693690492</v>
       </c>
       <c r="E102" t="n">
-        <v>0.06352559925996507</v>
+        <v>0.007826706456595304</v>
       </c>
       <c r="F102" t="n">
-        <v>0.2390625031117363</v>
+        <v>0.2398155597098134</v>
       </c>
       <c r="G102" t="n">
-        <v>0.1322389405010349</v>
+        <v>0.1309882148724703</v>
       </c>
       <c r="H102" t="n">
-        <v>0.3284764792675501</v>
+        <v>0.3175424841073513</v>
       </c>
       <c r="I102" t="n">
-        <v>0.03601083649481494</v>
+        <v>0.04306482958905249</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="inlineStr">
-        <is>
-          <t>Haysi, VA</t>
-        </is>
+      <c r="A103" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B103" t="n">
         <v>82.29583</v>
@@ -3619,29 +3415,27 @@
         <v>37.20694</v>
       </c>
       <c r="D103" t="n">
-        <v>0.2579585078069113</v>
+        <v>0.3302705346683392</v>
       </c>
       <c r="E103" t="n">
-        <v>0.1034503645224316</v>
+        <v>0.03494939665621741</v>
       </c>
       <c r="F103" t="n">
-        <v>0.2168294883544121</v>
+        <v>0.2143035011504664</v>
       </c>
       <c r="G103" t="n">
-        <v>0.1732882319859365</v>
+        <v>0.1784740572327244</v>
       </c>
       <c r="H103" t="n">
-        <v>0.3406021747895733</v>
+        <v>0.3279625816639743</v>
       </c>
       <c r="I103" t="n">
-        <v>0.02932481107257092</v>
+        <v>0.03631969873660307</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="inlineStr">
-        <is>
-          <t>Clintwood, VA</t>
-        </is>
+      <c r="A104" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B104" t="n">
         <v>82.43889</v>
@@ -3650,29 +3444,27 @@
         <v>37.12389</v>
       </c>
       <c r="D104" t="n">
-        <v>0.2460688819560911</v>
+        <v>0.2978278774664994</v>
       </c>
       <c r="E104" t="n">
-        <v>0.1209406184305275</v>
+        <v>0.05859466127906716</v>
       </c>
       <c r="F104" t="n">
-        <v>0.1407380542230375</v>
+        <v>0.1332000556847192</v>
       </c>
       <c r="G104" t="n">
-        <v>0.3801204607536621</v>
+        <v>0.406409195746768</v>
       </c>
       <c r="H104" t="n">
-        <v>0.2616881243286762</v>
+        <v>0.2481244903123814</v>
       </c>
       <c r="I104" t="n">
-        <v>0.09838277406783248</v>
+        <v>0.1177676874418562</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="inlineStr">
-        <is>
-          <t>Haysi, VA1</t>
-        </is>
+      <c r="A105" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B105" t="n">
         <v>82.34332999999999</v>
@@ -3681,29 +3473,27 @@
         <v>37.23694</v>
       </c>
       <c r="D105" t="n">
-        <v>0.3041053586483986</v>
+        <v>0.341059410814476</v>
       </c>
       <c r="E105" t="n">
-        <v>0.05322827982956899</v>
+        <v>0.02909430034528448</v>
       </c>
       <c r="F105" t="n">
-        <v>0.1649140312070574</v>
+        <v>0.1589708939564953</v>
       </c>
       <c r="G105" t="n">
-        <v>0.3028292206574021</v>
+        <v>0.3208255775467041</v>
       </c>
       <c r="H105" t="n">
-        <v>0.3238398540046542</v>
+        <v>0.310465029482324</v>
       </c>
       <c r="I105" t="n">
-        <v>0.0388768461907733</v>
+        <v>0.0482012481638236</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="inlineStr">
-        <is>
-          <t>Williamson, WV</t>
-        </is>
+      <c r="A106" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B106" t="n">
         <v>82.28028</v>
@@ -3712,29 +3502,27 @@
         <v>37.67306</v>
       </c>
       <c r="D106" t="n">
-        <v>0.2734665864522727</v>
+        <v>0.3826826985717404</v>
       </c>
       <c r="E106" t="n">
-        <v>0.08362341153661224</v>
+        <v>0.01353426920313306</v>
       </c>
       <c r="F106" t="n">
-        <v>0.2303503128311492</v>
+        <v>0.2257143851028771</v>
       </c>
       <c r="G106" t="n">
-        <v>0.1473613132490428</v>
+        <v>0.1559081255089136</v>
       </c>
       <c r="H106" t="n">
-        <v>0.2752417307023513</v>
+        <v>0.2609792500305201</v>
       </c>
       <c r="I106" t="n">
-        <v>0.08155707361019304</v>
+        <v>0.0993309891460203</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="inlineStr">
-        <is>
-          <t>Greenup, KY</t>
-        </is>
+      <c r="A107" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B107" t="n">
         <v>82.95222</v>
@@ -3743,29 +3531,27 @@
         <v>38.56417</v>
       </c>
       <c r="D107" t="n">
-        <v>0.2844996501913444</v>
+        <v>0.3443995879061786</v>
       </c>
       <c r="E107" t="n">
-        <v>0.07141815172489198</v>
+        <v>0.02745543374153369</v>
       </c>
       <c r="F107" t="n">
-        <v>0.2721671093098942</v>
+        <v>0.2704047238391584</v>
       </c>
       <c r="G107" t="n">
-        <v>0.08516170600546372</v>
+        <v>0.08728300071866191</v>
       </c>
       <c r="H107" t="n">
-        <v>0.09701559307748689</v>
+        <v>0.08565857800506221</v>
       </c>
       <c r="I107" t="n">
-        <v>0.5462305576569059</v>
+        <v>0.5943791124586523</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="inlineStr">
-        <is>
-          <t>West Union, OH</t>
-        </is>
+      <c r="A108" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B108" t="n">
         <v>83.42111</v>
@@ -3774,29 +3560,27 @@
         <v>38.80361</v>
       </c>
       <c r="D108" t="n">
-        <v>0.1670619030311744</v>
+        <v>0.2010889555744552</v>
       </c>
       <c r="E108" t="n">
-        <v>0.2964872359560941</v>
+        <v>0.2074158912302252</v>
       </c>
       <c r="F108" t="n">
-        <v>0.08788927008892683</v>
+        <v>0.08684169549386619</v>
       </c>
       <c r="G108" t="n">
-        <v>0.5847762682184873</v>
+        <v>0.5892773111976977</v>
       </c>
       <c r="H108" t="n">
-        <v>0.04129805543728893</v>
+        <v>0.0362444888642539</v>
       </c>
       <c r="I108" t="n">
-        <v>0.7976666193782598</v>
+        <v>0.8219989628575959</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="inlineStr">
-        <is>
-          <t>Wooton, KY</t>
-        </is>
+      <c r="A109" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B109" t="n">
         <v>83.30806</v>
@@ -3805,29 +3589,27 @@
         <v>37.165</v>
       </c>
       <c r="D109" t="n">
-        <v>0.2524871828100023</v>
+        <v>0.3062270300661588</v>
       </c>
       <c r="E109" t="n">
-        <v>0.1112421133403975</v>
+        <v>0.05150644903507222</v>
       </c>
       <c r="F109" t="n">
-        <v>-0.03160414037762314</v>
+        <v>-0.03731262088701257</v>
       </c>
       <c r="G109" t="n">
-        <v>0.8444881435508437</v>
+        <v>0.8168414812540438</v>
       </c>
       <c r="H109" t="n">
-        <v>0.3385325142279898</v>
+        <v>0.3307890961785754</v>
       </c>
       <c r="I109" t="n">
-        <v>0.03038717076436842</v>
+        <v>0.03464742031442954</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="inlineStr">
-        <is>
-          <t>Tallega, KY</t>
-        </is>
+      <c r="A110" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B110" t="n">
         <v>83.59389</v>
@@ -3836,29 +3618,27 @@
         <v>37.555</v>
       </c>
       <c r="D110" t="n">
-        <v>0.2853450403728114</v>
+        <v>0.3390886881746224</v>
       </c>
       <c r="E110" t="n">
-        <v>0.07054416736041852</v>
+        <v>0.0300986127445763</v>
       </c>
       <c r="F110" t="n">
-        <v>-0.03116411994358118</v>
+        <v>-0.03855712499005473</v>
       </c>
       <c r="G110" t="n">
-        <v>0.8466273067162603</v>
+        <v>0.8108419994395634</v>
       </c>
       <c r="H110" t="n">
-        <v>0.4023994188097236</v>
+        <v>0.3919323575111225</v>
       </c>
       <c r="I110" t="n">
-        <v>0.009101392258876595</v>
+        <v>0.01126781994188485</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="inlineStr">
-        <is>
-          <t>Heidelberg, KY</t>
-        </is>
+      <c r="A111" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B111" t="n">
         <v>83.76833000000001</v>
@@ -3867,29 +3647,27 @@
         <v>37.55528</v>
       </c>
       <c r="D111" t="n">
-        <v>0.3127731828079</v>
+        <v>0.3657697359955022</v>
       </c>
       <c r="E111" t="n">
-        <v>0.04647445493394614</v>
+        <v>0.01868361751283294</v>
       </c>
       <c r="F111" t="n">
-        <v>0.02151367016853553</v>
+        <v>0.01550696759721773</v>
       </c>
       <c r="G111" t="n">
-        <v>0.8937901170050665</v>
+        <v>0.9233394480600805</v>
       </c>
       <c r="H111" t="n">
-        <v>0.4015418974011961</v>
+        <v>0.3905205113116423</v>
       </c>
       <c r="I111" t="n">
-        <v>0.009264311843649479</v>
+        <v>0.01159124691925901</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="inlineStr">
-        <is>
-          <t>Rosman, NC</t>
-        </is>
+      <c r="A112" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B112" t="n">
         <v>82.82472</v>
@@ -3898,29 +3676,27 @@
         <v>35.14333</v>
       </c>
       <c r="D112" t="n">
-        <v>0.1075713927218527</v>
+        <v>0.1330757433466453</v>
       </c>
       <c r="E112" t="n">
-        <v>0.5032158184280278</v>
+        <v>0.4068512844480413</v>
       </c>
       <c r="F112" t="n">
-        <v>-0.002623251993274806</v>
+        <v>-0.006944742169800469</v>
       </c>
       <c r="G112" t="n">
-        <v>0.9870129559653125</v>
+        <v>0.9656271371304332</v>
       </c>
       <c r="H112" t="n">
-        <v>0.2170834665747125</v>
+        <v>0.2108650616554177</v>
       </c>
       <c r="I112" t="n">
-        <v>0.1727728695293844</v>
+        <v>0.1857101116556192</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="inlineStr">
-        <is>
-          <t>Blantyre, NC</t>
-        </is>
+      <c r="A113" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B113" t="n">
         <v>82.62389</v>
@@ -3929,29 +3705,27 @@
         <v>35.29917</v>
       </c>
       <c r="D113" t="n">
-        <v>0.08161254787689501</v>
+        <v>0.1120499148000216</v>
       </c>
       <c r="E113" t="n">
-        <v>0.6119709752311567</v>
+        <v>0.4855006869597325</v>
       </c>
       <c r="F113" t="n">
-        <v>-0.03909182102639883</v>
+        <v>-0.04358067525750849</v>
       </c>
       <c r="G113" t="n">
-        <v>0.8082676011689148</v>
+        <v>0.7867362421302553</v>
       </c>
       <c r="H113" t="n">
-        <v>0.1820395742037406</v>
+        <v>0.1770729409019236</v>
       </c>
       <c r="I113" t="n">
-        <v>0.2546513928860325</v>
+        <v>0.2680621031000459</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="1" t="inlineStr">
-        <is>
-          <t>Mills River, NC</t>
-        </is>
+      <c r="A114" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B114" t="n">
         <v>82.595</v>
@@ -3960,29 +3734,27 @@
         <v>35.39806</v>
       </c>
       <c r="D114" t="n">
-        <v>0.1127941797050099</v>
+        <v>0.1405124563022474</v>
       </c>
       <c r="E114" t="n">
-        <v>0.4825884695448228</v>
+        <v>0.3808923355410387</v>
       </c>
       <c r="F114" t="n">
-        <v>0.0007730863163750504</v>
+        <v>-0.003911850623258335</v>
       </c>
       <c r="G114" t="n">
-        <v>0.9961725007301013</v>
+        <v>0.9806344421374487</v>
       </c>
       <c r="H114" t="n">
-        <v>0.1936952825589874</v>
+        <v>0.1868916498894976</v>
       </c>
       <c r="I114" t="n">
-        <v>0.2249648562152189</v>
+        <v>0.2419904020830975</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="inlineStr">
-        <is>
-          <t>Biltmore, NC</t>
-        </is>
+      <c r="A115" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B115" t="n">
         <v>82.54472</v>
@@ -3991,29 +3763,27 @@
         <v>35.56833</v>
       </c>
       <c r="D115" t="n">
-        <v>0.2716084423671379</v>
+        <v>0.2845254108506861</v>
       </c>
       <c r="E115" t="n">
-        <v>0.08582976336228715</v>
+        <v>0.07139139440017041</v>
       </c>
       <c r="F115" t="n">
-        <v>0.1889840375974461</v>
+        <v>0.1843074230017637</v>
       </c>
       <c r="G115" t="n">
-        <v>0.23666420717145</v>
+        <v>0.2486796475662071</v>
       </c>
       <c r="H115" t="n">
-        <v>0.09536876705184825</v>
+        <v>0.08333155176760125</v>
       </c>
       <c r="I115" t="n">
-        <v>0.5530956583585016</v>
+        <v>0.6044697886402886</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="1" t="inlineStr">
-        <is>
-          <t>Asheville, NC</t>
-        </is>
+      <c r="A116" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B116" t="n">
         <v>82.57805999999999</v>
@@ -4022,29 +3792,27 @@
         <v>35.60889</v>
       </c>
       <c r="D116" t="n">
-        <v>0.1212846595533471</v>
+        <v>0.1562118806411244</v>
       </c>
       <c r="E116" t="n">
-        <v>0.450021497315125</v>
+        <v>0.3294035873258637</v>
       </c>
       <c r="F116" t="n">
-        <v>0.01072363788003597</v>
+        <v>0.006078454639825193</v>
       </c>
       <c r="G116" t="n">
-        <v>0.9469454090917105</v>
+        <v>0.9699127172311617</v>
       </c>
       <c r="H116" t="n">
-        <v>0.1852286697477298</v>
+        <v>0.1783038934505978</v>
       </c>
       <c r="I116" t="n">
-        <v>0.2462809053640845</v>
+        <v>0.2646956993638053</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="inlineStr">
-        <is>
-          <t>Hazelwood, NC</t>
-        </is>
+      <c r="A117" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B117" t="n">
         <v>82.9375</v>
@@ -4053,29 +3821,27 @@
         <v>35.39611</v>
       </c>
       <c r="D117" t="n">
-        <v>0.04177348849960863</v>
+        <v>0.05437355511882629</v>
       </c>
       <c r="E117" t="n">
-        <v>0.7953867770918279</v>
+        <v>0.7356318024580831</v>
       </c>
       <c r="F117" t="n">
-        <v>-0.06789606576908447</v>
+        <v>-0.07193397603635314</v>
       </c>
       <c r="G117" t="n">
-        <v>0.6731786170202289</v>
+        <v>0.6549200477320508</v>
       </c>
       <c r="H117" t="n">
-        <v>0.2141878908095034</v>
+        <v>0.2106280949093993</v>
       </c>
       <c r="I117" t="n">
-        <v>0.1787140301513994</v>
+        <v>0.1862163628372016</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="inlineStr">
-        <is>
-          <t>Canton, NC</t>
-        </is>
+      <c r="A118" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B118" t="n">
         <v>82.86972</v>
@@ -4084,29 +3850,27 @@
         <v>35.46167</v>
       </c>
       <c r="D118" t="n">
-        <v>0.08276994097031845</v>
+        <v>0.08890111956691561</v>
       </c>
       <c r="E118" t="n">
-        <v>0.6069161184313122</v>
+        <v>0.5804433674848433</v>
       </c>
       <c r="F118" t="n">
-        <v>-0.03527647292326752</v>
+        <v>-0.04025720999825863</v>
       </c>
       <c r="G118" t="n">
-        <v>0.8266794334016131</v>
+        <v>0.8026635505466001</v>
       </c>
       <c r="H118" t="n">
-        <v>0.2164838421900529</v>
+        <v>0.211009616265548</v>
       </c>
       <c r="I118" t="n">
-        <v>0.1739913756833193</v>
+        <v>0.1854017685713579</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="1" t="inlineStr">
-        <is>
-          <t>Cataloochee, NC</t>
-        </is>
+      <c r="A119" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B119" t="n">
         <v>83.07277999999999</v>
@@ -4115,29 +3879,27 @@
         <v>35.66722</v>
       </c>
       <c r="D119" t="n">
-        <v>0.06184370939742677</v>
+        <v>0.09972528029677002</v>
       </c>
       <c r="E119" t="n">
-        <v>0.7008933768843856</v>
+        <v>0.5350238323592295</v>
       </c>
       <c r="F119" t="n">
-        <v>-0.007927736709963426</v>
+        <v>-0.01190936224171468</v>
       </c>
       <c r="G119" t="n">
-        <v>0.9607653617250783</v>
+        <v>0.9410888496749943</v>
       </c>
       <c r="H119" t="n">
-        <v>0.3012488787352476</v>
+        <v>0.2951135826412459</v>
       </c>
       <c r="I119" t="n">
-        <v>0.05561907894078763</v>
+        <v>0.06104479050963445</v>
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="1" t="inlineStr">
-        <is>
-          <t>Celo, NC</t>
-        </is>
+      <c r="A120" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B120" t="n">
         <v>82.18416999999999</v>
@@ -4146,29 +3908,27 @@
         <v>35.83139</v>
       </c>
       <c r="D120" t="n">
-        <v>0.1198289418034575</v>
+        <v>0.1341737943527344</v>
       </c>
       <c r="E120" t="n">
-        <v>0.4555186287023213</v>
+        <v>0.4029558581082123</v>
       </c>
       <c r="F120" t="n">
-        <v>0.08553593338597076</v>
+        <v>0.08145605333961997</v>
       </c>
       <c r="G120" t="n">
-        <v>0.5949090845345595</v>
+        <v>0.6126558289708647</v>
       </c>
       <c r="H120" t="n">
-        <v>0.04339829232050972</v>
+        <v>0.03627767763204673</v>
       </c>
       <c r="I120" t="n">
-        <v>0.7876081341297106</v>
+        <v>0.8218385981917511</v>
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="1" t="inlineStr">
-        <is>
-          <t>Embreeville, TN</t>
-        </is>
+      <c r="A121" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B121" t="n">
         <v>82.4575</v>
@@ -4177,29 +3937,27 @@
         <v>36.17639</v>
       </c>
       <c r="D121" t="n">
-        <v>0.2169274169014757</v>
+        <v>0.2338208091836766</v>
       </c>
       <c r="E121" t="n">
-        <v>0.1730893886782554</v>
+        <v>0.1411920647537174</v>
       </c>
       <c r="F121" t="n">
-        <v>0.1680636685795492</v>
+        <v>0.1638048991349439</v>
       </c>
       <c r="G121" t="n">
-        <v>0.293558758679734</v>
+        <v>0.3061378158330187</v>
       </c>
       <c r="H121" t="n">
-        <v>0.161996968185459</v>
+        <v>0.1508031114693573</v>
       </c>
       <c r="I121" t="n">
-        <v>0.3115801178214944</v>
+        <v>0.3466297883077222</v>
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="inlineStr">
-        <is>
-          <t>Chilhowee, VA</t>
-        </is>
+      <c r="A122" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B122" t="n">
         <v>81.63139</v>
@@ -4208,29 +3966,27 @@
         <v>36.76028</v>
       </c>
       <c r="D122" t="n">
-        <v>0.2816885997601171</v>
+        <v>0.3523692809025185</v>
       </c>
       <c r="E122" t="n">
-        <v>0.07438572388634046</v>
+        <v>0.02385203997121885</v>
       </c>
       <c r="F122" t="n">
-        <v>0.141482925294941</v>
+        <v>0.13966475710197</v>
       </c>
       <c r="G122" t="n">
-        <v>0.3775784805630645</v>
+        <v>0.3838009627969658</v>
       </c>
       <c r="H122" t="n">
-        <v>0.3327276743954719</v>
+        <v>0.3223750973694852</v>
       </c>
       <c r="I122" t="n">
-        <v>0.0335374223325414</v>
+        <v>0.0398200025617491</v>
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="inlineStr">
-        <is>
-          <t>Damascus, VA</t>
-        </is>
+      <c r="A123" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B123" t="n">
         <v>81.84417000000001</v>
@@ -4239,29 +3995,27 @@
         <v>36.65167</v>
       </c>
       <c r="D123" t="n">
-        <v>0.3156706264195107</v>
+        <v>0.3719750906007967</v>
       </c>
       <c r="E123" t="n">
-        <v>0.04437798255524629</v>
+        <v>0.01663022266181372</v>
       </c>
       <c r="F123" t="n">
-        <v>0.2013801544766939</v>
+        <v>0.2012737801662148</v>
       </c>
       <c r="G123" t="n">
-        <v>0.2067448494287072</v>
+        <v>0.2069898037241473</v>
       </c>
       <c r="H123" t="n">
-        <v>0.2763415434092575</v>
+        <v>0.2659850422679193</v>
       </c>
       <c r="I123" t="n">
-        <v>0.08029695938315357</v>
+        <v>0.09278297241366321</v>
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="1" t="inlineStr">
-        <is>
-          <t>Sugar Grove, NC</t>
-        </is>
+      <c r="A124" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B124" t="n">
         <v>81.82222</v>
@@ -4270,29 +4024,27 @@
         <v>36.23917</v>
       </c>
       <c r="D124" t="n">
-        <v>0.2825435174041371</v>
+        <v>0.2761934914270414</v>
       </c>
       <c r="E124" t="n">
-        <v>0.07347313896632303</v>
+        <v>0.08046569973026392</v>
       </c>
       <c r="F124" t="n">
-        <v>0.1213676222328611</v>
+        <v>0.1182663199028734</v>
       </c>
       <c r="G124" t="n">
-        <v>0.4497093029372288</v>
+        <v>0.4614596391085138</v>
       </c>
       <c r="H124" t="n">
-        <v>0.3260048085949743</v>
+        <v>0.3155701893512519</v>
       </c>
       <c r="I124" t="n">
-        <v>0.03751629305975072</v>
+        <v>0.04444934904663246</v>
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="1" t="inlineStr">
-        <is>
-          <t>Saltville, VA</t>
-        </is>
+      <c r="A125" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B125" t="n">
         <v>81.74639000000001</v>
@@ -4301,29 +4053,27 @@
         <v>36.89667</v>
       </c>
       <c r="D125" t="n">
-        <v>0.2253959566077076</v>
+        <v>0.3123312612204821</v>
       </c>
       <c r="E125" t="n">
-        <v>0.1565081689772949</v>
+        <v>0.04680113751439098</v>
       </c>
       <c r="F125" t="n">
-        <v>0.1251541056222083</v>
+        <v>0.1274760484611864</v>
       </c>
       <c r="G125" t="n">
-        <v>0.4355867182575896</v>
+        <v>0.4270495991934899</v>
       </c>
       <c r="H125" t="n">
-        <v>0.3487192011682633</v>
+        <v>0.3425893318364445</v>
       </c>
       <c r="I125" t="n">
-        <v>0.0254501657140322</v>
+        <v>0.02833387352190867</v>
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="1" t="inlineStr">
-        <is>
-          <t>Maryville, TN</t>
-        </is>
+      <c r="A126" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B126" t="n">
         <v>83.8847</v>
@@ -4332,29 +4082,27 @@
         <v>35.78554</v>
       </c>
       <c r="D126" t="n">
-        <v>0.1173248829326039</v>
+        <v>0.1745425617865719</v>
       </c>
       <c r="E126" t="n">
-        <v>0.4650589101646731</v>
+        <v>0.275070593225003</v>
       </c>
       <c r="F126" t="n">
-        <v>-0.02764085009348019</v>
+        <v>-0.02661781264546365</v>
       </c>
       <c r="G126" t="n">
-        <v>0.8637936478328737</v>
+        <v>0.8687901265638874</v>
       </c>
       <c r="H126" t="n">
-        <v>0.4269301399374418</v>
+        <v>0.4243875257973556</v>
       </c>
       <c r="I126" t="n">
-        <v>0.00537305104584419</v>
+        <v>0.005684895208760445</v>
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="1" t="inlineStr">
-        <is>
-          <t>Prentiss, NC</t>
-        </is>
+      <c r="A127" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B127" t="n">
         <v>83.37972000000001</v>
@@ -4363,29 +4111,27 @@
         <v>35.15</v>
       </c>
       <c r="D127" t="n">
-        <v>0.0956851717555402</v>
+        <v>0.1347823795323213</v>
       </c>
       <c r="E127" t="n">
-        <v>0.5517735182667999</v>
+        <v>0.4008061359567318</v>
       </c>
       <c r="F127" t="n">
-        <v>-0.01197111933315964</v>
+        <v>-0.01656318934433076</v>
       </c>
       <c r="G127" t="n">
-        <v>0.9407838987081847</v>
+        <v>0.9181349723898882</v>
       </c>
       <c r="H127" t="n">
-        <v>0.2216222961725376</v>
+        <v>0.2156014292481272</v>
       </c>
       <c r="I127" t="n">
-        <v>0.1637477929100279</v>
+        <v>0.175795739225996</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="1" t="inlineStr">
-        <is>
-          <t>Rainbow Springs, NC</t>
-        </is>
+      <c r="A128" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B128" t="n">
         <v>83.61861</v>
@@ -4394,29 +4140,27 @@
         <v>37.1275</v>
       </c>
       <c r="D128" t="n">
-        <v>0.1251992374466721</v>
+        <v>0.1555563662591471</v>
       </c>
       <c r="E128" t="n">
-        <v>0.4354198854315452</v>
+        <v>0.3314624326156564</v>
       </c>
       <c r="F128" t="n">
-        <v>0.01877784941398394</v>
+        <v>0.01490765871639255</v>
       </c>
       <c r="G128" t="n">
-        <v>0.9072335433763173</v>
+        <v>0.9262939271808324</v>
       </c>
       <c r="H128" t="n">
-        <v>0.2988891749708247</v>
+        <v>0.2919275514209731</v>
       </c>
       <c r="I128" t="n">
-        <v>0.05765826263713353</v>
+        <v>0.06402401891332707</v>
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="1" t="inlineStr">
-        <is>
-          <t>Birdtown, NC</t>
-        </is>
+      <c r="A129" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B129" t="n">
         <v>83.35361</v>
@@ -4425,29 +4169,27 @@
         <v>35.46139</v>
       </c>
       <c r="D129" t="n">
-        <v>0.06321091642675551</v>
+        <v>0.1244889964743222</v>
       </c>
       <c r="E129" t="n">
-        <v>0.6945976139676063</v>
+        <v>0.4380494438295457</v>
       </c>
       <c r="F129" t="n">
-        <v>-0.07078703932302108</v>
+        <v>-0.07371827849124524</v>
       </c>
       <c r="G129" t="n">
-        <v>0.660086696439808</v>
+        <v>0.6469137782748178</v>
       </c>
       <c r="H129" t="n">
-        <v>0.3905050183842813</v>
+        <v>0.3861795357205758</v>
       </c>
       <c r="I129" t="n">
-        <v>0.01159483948490575</v>
+        <v>0.01263570104313499</v>
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="1" t="inlineStr">
-        <is>
-          <t>Cleveland, VA</t>
-        </is>
+      <c r="A130" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B130" t="n">
         <v>82.155</v>
@@ -4456,29 +4198,27 @@
         <v>36.94472</v>
       </c>
       <c r="D130" t="n">
-        <v>0.1972675255901945</v>
+        <v>0.2969615969053408</v>
       </c>
       <c r="E130" t="n">
-        <v>0.2163629823601105</v>
+        <v>0.05936795402015545</v>
       </c>
       <c r="F130" t="n">
-        <v>0.1263151475269076</v>
+        <v>0.1261842493303484</v>
       </c>
       <c r="G130" t="n">
-        <v>0.4313061313077957</v>
+        <v>0.4317875576793102</v>
       </c>
       <c r="H130" t="n">
-        <v>0.2891031127138874</v>
+        <v>0.2811927041409682</v>
       </c>
       <c r="I130" t="n">
-        <v>0.06676053662434604</v>
+        <v>0.07491913304674702</v>
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="1" t="inlineStr">
-        <is>
-          <t>Jonesville, VA</t>
-        </is>
+      <c r="A131" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B131" t="n">
         <v>83.095</v>
@@ -4487,29 +4227,27 @@
         <v>36.66194</v>
       </c>
       <c r="D131" t="n">
-        <v>0.3099203244942661</v>
+        <v>0.3494880385237609</v>
       </c>
       <c r="E131" t="n">
-        <v>0.04861621710725961</v>
+        <v>0.02510634465229246</v>
       </c>
       <c r="F131" t="n">
-        <v>0.07917920974170986</v>
+        <v>0.07501684432027725</v>
       </c>
       <c r="G131" t="n">
-        <v>0.6226563294975225</v>
+        <v>0.6411115652566726</v>
       </c>
       <c r="H131" t="n">
-        <v>0.3608122523391081</v>
+        <v>0.3501510212276927</v>
       </c>
       <c r="I131" t="n">
-        <v>0.02047351752661144</v>
+        <v>0.0248129715173694</v>
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="1" t="inlineStr">
-        <is>
-          <t>Tomotla, NC</t>
-        </is>
+      <c r="A132" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B132" t="n">
         <v>83.98056</v>
@@ -4518,22 +4256,22 @@
         <v>35.13889</v>
       </c>
       <c r="D132" t="n">
-        <v>0.1873995866151326</v>
+        <v>0.2537134227865898</v>
       </c>
       <c r="E132" t="n">
-        <v>0.2406900583246359</v>
+        <v>0.1094582733698106</v>
       </c>
       <c r="F132" t="n">
-        <v>0.02818004374488763</v>
+        <v>0.03038163974494858</v>
       </c>
       <c r="G132" t="n">
-        <v>0.8611623373658227</v>
+        <v>0.8504340159303216</v>
       </c>
       <c r="H132" t="n">
-        <v>0.4416008368223865</v>
+        <v>0.4382215808006398</v>
       </c>
       <c r="I132" t="n">
-        <v>0.003847642916741141</v>
+        <v>0.00416064191641425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated file with station names
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -476,8 +476,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Franklin, WV</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>79.33806</v>
@@ -505,8 +507,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>0</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Petersburg, WV</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>79.17610999999999</v>
@@ -534,8 +538,10 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>0</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Brandywine, WV</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>79.24666999999999</v>
@@ -563,8 +569,10 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>0</v>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Stokesville, VA</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>79.23917</v>
@@ -592,8 +600,10 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>0</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Bacova, VA</t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>79.88167</v>
@@ -621,8 +631,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>0</v>
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Sunrise, VA</t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>79.76889</v>
@@ -650,8 +662,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>0</v>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Hot Springs, VA</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>79.94944</v>
@@ -679,8 +693,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>0</v>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Covington, VA</t>
+        </is>
       </c>
       <c r="B9" t="n">
         <v>80.04722</v>
@@ -708,8 +724,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>0</v>
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Covington, VA1</t>
+        </is>
       </c>
       <c r="B10" t="n">
         <v>80.00082999999999</v>
@@ -737,8 +755,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>0</v>
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Covington, VA2</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>80.0425</v>
@@ -766,8 +786,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>0</v>
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Williamsville, VA</t>
+        </is>
       </c>
       <c r="B12" t="n">
         <v>79.57028</v>
@@ -795,8 +817,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>0</v>
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Clifton Forge, VA</t>
+        </is>
       </c>
       <c r="B13" t="n">
         <v>79.75972</v>
@@ -824,8 +848,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>0</v>
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Lick Run, VA</t>
+        </is>
       </c>
       <c r="B14" t="n">
         <v>79.78471999999999</v>
@@ -853,8 +879,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>0</v>
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>New Castle, VA</t>
+        </is>
       </c>
       <c r="B15" t="n">
         <v>80.10693999999999</v>
@@ -882,8 +910,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>0</v>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Parr, VA</t>
+        </is>
       </c>
       <c r="B16" t="n">
         <v>79.90889</v>
@@ -911,8 +941,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>0</v>
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Catawba, VA</t>
+        </is>
       </c>
       <c r="B17" t="n">
         <v>80.00556</v>
@@ -940,8 +972,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>0</v>
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Buchanan, VA</t>
+        </is>
       </c>
       <c r="B18" t="n">
         <v>79.67917</v>
@@ -969,8 +1003,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>0</v>
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>Rockbridge Baths, VA</t>
+        </is>
       </c>
       <c r="B19" t="n">
         <v>79.42222</v>
@@ -998,8 +1034,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>0</v>
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>Lexington, VA</t>
+        </is>
       </c>
       <c r="B20" t="n">
         <v>79.44333</v>
@@ -1027,8 +1065,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>0</v>
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Buena Vista, VA</t>
+        </is>
       </c>
       <c r="B21" t="n">
         <v>79.39167</v>
@@ -1056,8 +1096,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>0</v>
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Holcomb Rock, VA</t>
+        </is>
       </c>
       <c r="B22" t="n">
         <v>79.26278000000001</v>
@@ -1085,8 +1127,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>0</v>
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>Piney River, VA</t>
+        </is>
       </c>
       <c r="B23" t="n">
         <v>79.02778000000001</v>
@@ -1114,8 +1158,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>0</v>
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Shawsville, VA</t>
+        </is>
       </c>
       <c r="B24" t="n">
         <v>80.26667</v>
@@ -1143,8 +1189,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>0</v>
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>Lafayette, VA</t>
+        </is>
       </c>
       <c r="B25" t="n">
         <v>80.20944</v>
@@ -1172,8 +1220,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>0</v>
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Roanoke, VA</t>
+        </is>
       </c>
       <c r="B26" t="n">
         <v>79.93889</v>
@@ -1201,8 +1251,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>0</v>
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>Niagara, VA</t>
+        </is>
       </c>
       <c r="B27" t="n">
         <v>79.87166999999999</v>
@@ -1230,8 +1282,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>0</v>
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>Dundee, VA</t>
+        </is>
       </c>
       <c r="B28" t="n">
         <v>79.86833</v>
@@ -1259,8 +1313,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>0</v>
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>Rocky Mount, VA</t>
+        </is>
       </c>
       <c r="B29" t="n">
         <v>79.84444000000001</v>
@@ -1288,8 +1344,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>0</v>
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>Sandy Level, VA</t>
+        </is>
       </c>
       <c r="B30" t="n">
         <v>79.52500000000001</v>
@@ -1317,8 +1375,10 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>0</v>
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>Huddleston, VA</t>
+        </is>
       </c>
       <c r="B31" t="n">
         <v>79.52056</v>
@@ -1346,8 +1406,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>0</v>
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>Evington, VA</t>
+        </is>
       </c>
       <c r="B32" t="n">
         <v>79.30389</v>
@@ -1375,8 +1437,10 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>0</v>
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>Francisco, NC</t>
+        </is>
       </c>
       <c r="B33" t="n">
         <v>80.30306</v>
@@ -1404,8 +1468,10 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>0</v>
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>Nettleridge, VA</t>
+        </is>
       </c>
       <c r="B34" t="n">
         <v>80.12972000000001</v>
@@ -1433,8 +1499,10 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>0</v>
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>Spencer, VA</t>
+        </is>
       </c>
       <c r="B35" t="n">
         <v>79.9875</v>
@@ -1462,8 +1530,10 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>0</v>
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>Wentworth, NC</t>
+        </is>
       </c>
       <c r="B36" t="n">
         <v>79.82611</v>
@@ -1491,8 +1561,10 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>0</v>
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>Philpott, VA</t>
+        </is>
       </c>
       <c r="B37" t="n">
         <v>80.02500000000001</v>
@@ -1520,8 +1592,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>0</v>
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>Bassett, VA</t>
+        </is>
       </c>
       <c r="B38" t="n">
         <v>80.00111</v>
@@ -1549,8 +1623,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>0</v>
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Martinsville, VA</t>
+        </is>
       </c>
       <c r="B39" t="n">
         <v>79.88083</v>
@@ -1578,8 +1654,10 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>0</v>
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>Eden, NC</t>
+        </is>
       </c>
       <c r="B40" t="n">
         <v>79.76555999999999</v>
@@ -1607,8 +1685,10 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>0</v>
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>Danville, VA</t>
+        </is>
       </c>
       <c r="B41" t="n">
         <v>79.50444</v>
@@ -1636,8 +1716,10 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>0</v>
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>Paces, VA</t>
+        </is>
       </c>
       <c r="B42" t="n">
         <v>79.08972</v>
@@ -1665,8 +1747,10 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>0</v>
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>Leasburg, NC</t>
+        </is>
       </c>
       <c r="B43" t="n">
         <v>79.19667</v>
@@ -1694,8 +1778,10 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>0</v>
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>Bynum, NC</t>
+        </is>
       </c>
       <c r="B44" t="n">
         <v>79.13583</v>
@@ -1723,8 +1809,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>0</v>
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>Ramseur, NC</t>
+        </is>
       </c>
       <c r="B45" t="n">
         <v>79.65555999999999</v>
@@ -1752,8 +1840,10 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>0</v>
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>Moncure, NC</t>
+        </is>
       </c>
       <c r="B46" t="n">
         <v>79.11611000000001</v>
@@ -1781,8 +1871,10 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>0</v>
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>Iverness, NC</t>
+        </is>
       </c>
       <c r="B47" t="n">
         <v>79.17749999999999</v>
@@ -1810,8 +1902,10 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>0</v>
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>Patterson, NC</t>
+        </is>
       </c>
       <c r="B48" t="n">
         <v>81.55833</v>
@@ -1839,8 +1933,10 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>0</v>
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>Wilkesboro, NC</t>
+        </is>
       </c>
       <c r="B49" t="n">
         <v>81.16889</v>
@@ -1868,8 +1964,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>0</v>
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>Wilkesboro, NC 1</t>
+        </is>
       </c>
       <c r="B50" t="n">
         <v>81.14556</v>
@@ -1897,8 +1995,10 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>0</v>
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>Elkin, NC</t>
+        </is>
       </c>
       <c r="B51" t="n">
         <v>80.84911</v>
@@ -1926,8 +2026,10 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>0</v>
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>Ararat, NC</t>
+        </is>
       </c>
       <c r="B52" t="n">
         <v>80.56169</v>
@@ -1955,8 +2057,10 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>0</v>
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>Dalton, NC</t>
+        </is>
       </c>
       <c r="B53" t="n">
         <v>80.41472</v>
@@ -1984,8 +2088,10 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>0</v>
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>Enon, NC</t>
+        </is>
       </c>
       <c r="B54" t="n">
         <v>80.44528</v>
@@ -2013,8 +2119,10 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>0</v>
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>Mocksville, NC</t>
+        </is>
       </c>
       <c r="B55" t="n">
         <v>80.65889</v>
@@ -2042,8 +2150,10 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>0</v>
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>Barber, NC</t>
+        </is>
       </c>
       <c r="B56" t="n">
         <v>80.59607</v>
@@ -2071,8 +2181,10 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>0</v>
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>Norwood, NC</t>
+        </is>
       </c>
       <c r="B57" t="n">
         <v>80.16576999999999</v>
@@ -2100,8 +2212,10 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>0</v>
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>Rockingham, NC</t>
+        </is>
       </c>
       <c r="B58" t="n">
         <v>79.86972</v>
@@ -2129,8 +2243,10 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>0</v>
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>Mcbee, SC</t>
+        </is>
       </c>
       <c r="B59" t="n">
         <v>80.18333</v>
@@ -2158,8 +2274,10 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>0</v>
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>Hartsville, SC</t>
+        </is>
       </c>
       <c r="B60" t="n">
         <v>80.15000000000001</v>
@@ -2187,8 +2305,10 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>0</v>
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>Effingham, SC</t>
+        </is>
       </c>
       <c r="B61" t="n">
         <v>79.75417</v>
@@ -2216,8 +2336,10 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>0</v>
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>Hoffman, NC</t>
+        </is>
       </c>
       <c r="B62" t="n">
         <v>79.49388999999999</v>
@@ -2245,8 +2367,10 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>0</v>
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>Nebo, NC</t>
+        </is>
       </c>
       <c r="B63" t="n">
         <v>81.89111</v>
@@ -2274,8 +2398,10 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>0</v>
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>Henry River, NC</t>
+        </is>
       </c>
       <c r="B64" t="n">
         <v>81.40333</v>
@@ -2303,8 +2429,10 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>0</v>
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>Ramsey, NC</t>
+        </is>
       </c>
       <c r="B65" t="n">
         <v>81.56694</v>
@@ -2332,8 +2460,10 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="n">
-        <v>0</v>
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>Laboratory, NC</t>
+        </is>
       </c>
       <c r="B66" t="n">
         <v>81.26528</v>
@@ -2361,8 +2491,10 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>0</v>
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>Bessemer City, NC</t>
+        </is>
       </c>
       <c r="B67" t="n">
         <v>81.23472</v>
@@ -2390,8 +2522,10 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>0</v>
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>Charlotte, NC</t>
+        </is>
       </c>
       <c r="B68" t="n">
         <v>80.85778000000001</v>
@@ -2419,8 +2553,10 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>0</v>
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>Charlotte, NC 1</t>
+        </is>
       </c>
       <c r="B69" t="n">
         <v>80.7675</v>
@@ -2448,8 +2584,10 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>0</v>
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>Lake Lure, NC</t>
+        </is>
       </c>
       <c r="B70" t="n">
         <v>82.11167</v>
@@ -2477,8 +2615,10 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>0</v>
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>Boiling Springs, NC</t>
+        </is>
       </c>
       <c r="B71" t="n">
         <v>81.69750000000001</v>
@@ -2506,8 +2646,10 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>0</v>
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>Casar, NC</t>
+        </is>
       </c>
       <c r="B72" t="n">
         <v>81.68222</v>
@@ -2535,8 +2677,10 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="n">
-        <v>0</v>
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>Fingerville, SC</t>
+        </is>
       </c>
       <c r="B73" t="n">
         <v>81.98611</v>
@@ -2564,8 +2708,10 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>0</v>
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>Carlisle, SC</t>
+        </is>
       </c>
       <c r="B74" t="n">
         <v>81.42139</v>
@@ -2593,8 +2739,10 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>0</v>
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>Delta, SC</t>
+        </is>
       </c>
       <c r="B75" t="n">
         <v>81.54833000000001</v>
@@ -2622,8 +2770,10 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>0</v>
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>Whitmire, SC</t>
+        </is>
       </c>
       <c r="B76" t="n">
         <v>81.59833</v>
@@ -2651,8 +2801,10 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>0</v>
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>Ware Shoals, SC</t>
+        </is>
       </c>
       <c r="B77" t="n">
         <v>82.22360999999999</v>
@@ -2680,8 +2832,10 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="n">
-        <v>0</v>
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>Chappels, SC</t>
+        </is>
       </c>
       <c r="B78" t="n">
         <v>81.86417</v>
@@ -2709,8 +2863,10 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>0</v>
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>Clayton, GA</t>
+        </is>
       </c>
       <c r="B79" t="n">
         <v>83.30611</v>
@@ -2738,8 +2894,10 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>0</v>
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>Clayton, GA 1</t>
+        </is>
       </c>
       <c r="B80" t="n">
         <v>83.53064000000001</v>
@@ -2767,8 +2925,10 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="n">
-        <v>0</v>
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>Cornelia, GA</t>
+        </is>
       </c>
       <c r="B81" t="n">
         <v>83.62277</v>
@@ -2796,8 +2956,10 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="n">
-        <v>0</v>
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>Jefferson, NC</t>
+        </is>
       </c>
       <c r="B82" t="n">
         <v>81.40694000000001</v>
@@ -2825,8 +2987,10 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="n">
-        <v>0</v>
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>Galax, VA</t>
+        </is>
       </c>
       <c r="B83" t="n">
         <v>80.97917</v>
@@ -2854,8 +3018,10 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="n">
-        <v>0</v>
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>Allisonia, VA</t>
+        </is>
       </c>
       <c r="B84" t="n">
         <v>80.74583</v>
@@ -2883,8 +3049,10 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="n">
-        <v>0</v>
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>Graysontown, VA</t>
+        </is>
       </c>
       <c r="B85" t="n">
         <v>80.55694</v>
@@ -2912,8 +3080,10 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="n">
-        <v>0</v>
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>Radford, VA</t>
+        </is>
       </c>
       <c r="B86" t="n">
         <v>80.56944</v>
@@ -2941,8 +3111,10 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="n">
-        <v>0</v>
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>Bane, VA</t>
+        </is>
       </c>
       <c r="B87" t="n">
         <v>80.70972</v>
@@ -2970,8 +3142,10 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="n">
-        <v>0</v>
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>Glen Lyn, VA</t>
+        </is>
       </c>
       <c r="B88" t="n">
         <v>80.86083000000001</v>
@@ -2999,8 +3173,10 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1" t="n">
-        <v>0</v>
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>Durbin, WV</t>
+        </is>
       </c>
       <c r="B89" t="n">
         <v>79.83333</v>
@@ -3028,8 +3204,10 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="1" t="n">
-        <v>0</v>
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>Buckeye, WV</t>
+        </is>
       </c>
       <c r="B90" t="n">
         <v>80.13</v>
@@ -3057,8 +3235,10 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="n">
-        <v>0</v>
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>Alderson, WV</t>
+        </is>
       </c>
       <c r="B91" t="n">
         <v>80.64167</v>
@@ -3086,8 +3266,10 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="n">
-        <v>0</v>
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>Hilldale, WV</t>
+        </is>
       </c>
       <c r="B92" t="n">
         <v>80.80528</v>
@@ -3115,8 +3297,10 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="n">
-        <v>0</v>
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>Dyer, WV</t>
+        </is>
       </c>
       <c r="B93" t="n">
         <v>80.48417000000001</v>
@@ -3144,8 +3328,10 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="n">
-        <v>0</v>
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>Belva, WV</t>
+        </is>
       </c>
       <c r="B94" t="n">
         <v>81.18111</v>
@@ -3173,8 +3359,10 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="1" t="n">
-        <v>0</v>
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>Kanawha Falls, WV</t>
+        </is>
       </c>
       <c r="B95" t="n">
         <v>81.21444</v>
@@ -3202,8 +3390,10 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="n">
-        <v>0</v>
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>Queen Shoals, WV</t>
+        </is>
       </c>
       <c r="B96" t="n">
         <v>81.28417</v>
@@ -3231,8 +3421,10 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="n">
-        <v>0</v>
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>Ashford, WV</t>
+        </is>
       </c>
       <c r="B97" t="n">
         <v>81.71167</v>
@@ -3260,8 +3452,10 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="n">
-        <v>0</v>
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>Tornado, WV</t>
+        </is>
       </c>
       <c r="B98" t="n">
         <v>81.84166999999999</v>
@@ -3289,8 +3483,10 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="n">
-        <v>0</v>
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>Baileysville, WV</t>
+        </is>
       </c>
       <c r="B99" t="n">
         <v>81.64528</v>
@@ -3318,8 +3514,10 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="n">
-        <v>0</v>
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>Clear Fork, WV</t>
+        </is>
       </c>
       <c r="B100" t="n">
         <v>81.7075</v>
@@ -3347,8 +3545,10 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="1" t="n">
-        <v>0</v>
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>Logan, WV</t>
+        </is>
       </c>
       <c r="B101" t="n">
         <v>81.97611000000001</v>
@@ -3376,8 +3576,10 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="n">
-        <v>0</v>
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>Big Rock, VA</t>
+        </is>
       </c>
       <c r="B102" t="n">
         <v>82.19583</v>
@@ -3405,8 +3607,10 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="n">
-        <v>0</v>
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>Haysi, VA</t>
+        </is>
       </c>
       <c r="B103" t="n">
         <v>82.29583</v>
@@ -3434,8 +3638,10 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="n">
-        <v>0</v>
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>Clintwood, VA</t>
+        </is>
       </c>
       <c r="B104" t="n">
         <v>82.43889</v>
@@ -3463,8 +3669,10 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>0</v>
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>Haysi, VA1</t>
+        </is>
       </c>
       <c r="B105" t="n">
         <v>82.34332999999999</v>
@@ -3492,8 +3700,10 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>0</v>
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>Williamson, WV</t>
+        </is>
       </c>
       <c r="B106" t="n">
         <v>82.28028</v>
@@ -3521,8 +3731,10 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>0</v>
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>Greenup, KY</t>
+        </is>
       </c>
       <c r="B107" t="n">
         <v>82.95222</v>
@@ -3550,8 +3762,10 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>0</v>
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>West Union, OH</t>
+        </is>
       </c>
       <c r="B108" t="n">
         <v>83.42111</v>
@@ -3579,8 +3793,10 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>0</v>
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t>Wooton, KY</t>
+        </is>
       </c>
       <c r="B109" t="n">
         <v>83.30806</v>
@@ -3608,8 +3824,10 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>0</v>
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>Tallega, KY</t>
+        </is>
       </c>
       <c r="B110" t="n">
         <v>83.59389</v>
@@ -3637,8 +3855,10 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>0</v>
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>Heidelberg, KY</t>
+        </is>
       </c>
       <c r="B111" t="n">
         <v>83.76833000000001</v>
@@ -3666,8 +3886,10 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>0</v>
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>Rosman, NC</t>
+        </is>
       </c>
       <c r="B112" t="n">
         <v>82.82472</v>
@@ -3695,8 +3917,10 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>0</v>
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>Blantyre, NC</t>
+        </is>
       </c>
       <c r="B113" t="n">
         <v>82.62389</v>
@@ -3724,8 +3948,10 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>0</v>
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t>Mills River, NC</t>
+        </is>
       </c>
       <c r="B114" t="n">
         <v>82.595</v>
@@ -3753,8 +3979,10 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>0</v>
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>Biltmore, NC</t>
+        </is>
       </c>
       <c r="B115" t="n">
         <v>82.54472</v>
@@ -3782,8 +4010,10 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>0</v>
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t>Asheville, NC</t>
+        </is>
       </c>
       <c r="B116" t="n">
         <v>82.57805999999999</v>
@@ -3811,8 +4041,10 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>0</v>
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>Hazelwood, NC</t>
+        </is>
       </c>
       <c r="B117" t="n">
         <v>82.9375</v>
@@ -3840,8 +4072,10 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="n">
-        <v>0</v>
+      <c r="A118" s="1" t="inlineStr">
+        <is>
+          <t>Canton, NC</t>
+        </is>
       </c>
       <c r="B118" t="n">
         <v>82.86972</v>
@@ -3869,8 +4103,10 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="1" t="n">
-        <v>0</v>
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>Cataloochee, NC</t>
+        </is>
       </c>
       <c r="B119" t="n">
         <v>83.07277999999999</v>
@@ -3898,8 +4134,10 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="1" t="n">
-        <v>0</v>
+      <c r="A120" s="1" t="inlineStr">
+        <is>
+          <t>Celo, NC</t>
+        </is>
       </c>
       <c r="B120" t="n">
         <v>82.18416999999999</v>
@@ -3927,8 +4165,10 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="1" t="n">
-        <v>0</v>
+      <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t>Embreeville, TN</t>
+        </is>
       </c>
       <c r="B121" t="n">
         <v>82.4575</v>
@@ -3956,8 +4196,10 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="n">
-        <v>0</v>
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>Chilhowee, VA</t>
+        </is>
       </c>
       <c r="B122" t="n">
         <v>81.63139</v>
@@ -3985,8 +4227,10 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>0</v>
+      <c r="A123" s="1" t="inlineStr">
+        <is>
+          <t>Damascus, VA</t>
+        </is>
       </c>
       <c r="B123" t="n">
         <v>81.84417000000001</v>
@@ -4014,8 +4258,10 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="1" t="n">
-        <v>0</v>
+      <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t>Sugar Grove, NC</t>
+        </is>
       </c>
       <c r="B124" t="n">
         <v>81.82222</v>
@@ -4043,8 +4289,10 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="1" t="n">
-        <v>0</v>
+      <c r="A125" s="1" t="inlineStr">
+        <is>
+          <t>Saltville, VA</t>
+        </is>
       </c>
       <c r="B125" t="n">
         <v>81.74639000000001</v>
@@ -4072,8 +4320,10 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="1" t="n">
-        <v>0</v>
+      <c r="A126" s="1" t="inlineStr">
+        <is>
+          <t>Maryville, TN</t>
+        </is>
       </c>
       <c r="B126" t="n">
         <v>83.8847</v>
@@ -4101,8 +4351,10 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="1" t="n">
-        <v>0</v>
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>Prentiss, NC</t>
+        </is>
       </c>
       <c r="B127" t="n">
         <v>83.37972000000001</v>
@@ -4130,8 +4382,10 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="1" t="n">
-        <v>0</v>
+      <c r="A128" s="1" t="inlineStr">
+        <is>
+          <t>Rainbow Springs, NC</t>
+        </is>
       </c>
       <c r="B128" t="n">
         <v>83.61861</v>
@@ -4159,8 +4413,10 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="1" t="n">
-        <v>0</v>
+      <c r="A129" s="1" t="inlineStr">
+        <is>
+          <t>Birdtown, NC</t>
+        </is>
       </c>
       <c r="B129" t="n">
         <v>83.35361</v>
@@ -4188,8 +4444,10 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="1" t="n">
-        <v>0</v>
+      <c r="A130" s="1" t="inlineStr">
+        <is>
+          <t>Cleveland, VA</t>
+        </is>
       </c>
       <c r="B130" t="n">
         <v>82.155</v>
@@ -4217,8 +4475,10 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="1" t="n">
-        <v>0</v>
+      <c r="A131" s="1" t="inlineStr">
+        <is>
+          <t>Jonesville, VA</t>
+        </is>
       </c>
       <c r="B131" t="n">
         <v>83.095</v>
@@ -4246,8 +4506,10 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="1" t="n">
-        <v>0</v>
+      <c r="A132" s="1" t="inlineStr">
+        <is>
+          <t>Tomotla, NC</t>
+        </is>
       </c>
       <c r="B132" t="n">
         <v>83.98056</v>

</xml_diff>